<commit_message>
tweaks to census dataset
</commit_message>
<xml_diff>
--- a/states_correlation_dataset.xlsx
+++ b/states_correlation_dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbcme\OneDrive\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbcme\OneDrive\Documentos\GitHub\data-vis-nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FCCCC8-A764-464C-8907-AE584C90077F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BFEE7D-C7C3-4424-B3C7-DD97981A59E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B280968C-2C0A-420C-A93E-E5F0EEDC2270}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
   <si>
     <t>population</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t>selfempoyed</t>
+  </si>
+  <si>
+    <t>party_2020</t>
+  </si>
+  <si>
+    <t>REPUBLICAN</t>
+  </si>
+  <si>
+    <t>DEMOCRAT</t>
   </si>
 </sst>
 </file>
@@ -625,17 +634,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349CF4C0-C2B9-410F-AD99-9DA3A70DA3E4}">
-  <dimension ref="A1:AB52"/>
+  <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.34765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.34765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.84765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.09765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.94921875" style="1" customWidth="1"/>
@@ -658,10 +667,12 @@
     <col min="23" max="23" width="13.25" style="1" customWidth="1"/>
     <col min="24" max="24" width="22.19921875" style="1" customWidth="1"/>
     <col min="25" max="25" width="6.8984375" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.796875" style="1"/>
+    <col min="26" max="28" width="8.796875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -746,8 +757,11 @@
       <c r="AB1" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="AC1" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -832,8 +846,11 @@
       <c r="AB2" s="1">
         <v>5.18</v>
       </c>
+      <c r="AC2" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -918,8 +935,11 @@
       <c r="AB3" s="1">
         <v>7.08</v>
       </c>
+      <c r="AC3" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1004,8 +1024,11 @@
       <c r="AB4" s="1">
         <v>6.39</v>
       </c>
+      <c r="AC4" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1090,8 +1113,11 @@
       <c r="AB5" s="1">
         <v>6.31</v>
       </c>
+      <c r="AC5" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1176,8 +1202,11 @@
       <c r="AB6" s="1">
         <v>8.48</v>
       </c>
+      <c r="AC6" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1262,8 +1291,11 @@
       <c r="AB7" s="1">
         <v>6.67</v>
       </c>
+      <c r="AC7" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1348,8 +1380,11 @@
       <c r="AB8" s="1">
         <v>6.37</v>
       </c>
+      <c r="AC8" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1434,8 +1469,11 @@
       <c r="AB9" s="1">
         <v>4.0999999999999996</v>
       </c>
+      <c r="AC9" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1520,8 +1558,11 @@
       <c r="AB10" s="1">
         <v>4.1100000000000003</v>
       </c>
+      <c r="AC10" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1606,8 +1647,11 @@
       <c r="AB11" s="1">
         <v>6.3</v>
       </c>
+      <c r="AC11" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1692,8 +1736,11 @@
       <c r="AB12" s="1">
         <v>5.58</v>
       </c>
+      <c r="AC12" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1778,8 +1825,11 @@
       <c r="AB13" s="1">
         <v>7.27</v>
       </c>
+      <c r="AC13" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1864,8 +1914,11 @@
       <c r="AB14" s="1">
         <v>7.92</v>
       </c>
+      <c r="AC14" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1950,8 +2003,11 @@
       <c r="AB15" s="1">
         <v>4.74</v>
       </c>
+      <c r="AC15" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -2036,8 +2092,11 @@
       <c r="AB16" s="1">
         <v>4.6399999999999997</v>
       </c>
+      <c r="AC16" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -2122,8 +2181,11 @@
       <c r="AB17" s="1">
         <v>7.08</v>
       </c>
+      <c r="AC17" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2208,8 +2270,11 @@
       <c r="AB18" s="1">
         <v>6.66</v>
       </c>
+      <c r="AC18" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2294,8 +2359,11 @@
       <c r="AB19" s="1">
         <v>5.64</v>
       </c>
+      <c r="AC19" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2380,8 +2448,11 @@
       <c r="AB20" s="1">
         <v>5.78</v>
       </c>
+      <c r="AC20" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2466,8 +2537,11 @@
       <c r="AB21" s="1">
         <v>9.18</v>
       </c>
+      <c r="AC21" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2552,8 +2626,11 @@
       <c r="AB22" s="1">
         <v>4.88</v>
       </c>
+      <c r="AC22" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2638,8 +2715,11 @@
       <c r="AB23" s="1">
         <v>5.96</v>
       </c>
+      <c r="AC23" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2724,8 +2804,11 @@
       <c r="AB24" s="1">
         <v>5.04</v>
       </c>
+      <c r="AC24" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -2810,8 +2893,11 @@
       <c r="AB25" s="1">
         <v>5.88</v>
       </c>
+      <c r="AC25" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2896,8 +2982,11 @@
       <c r="AB26" s="1">
         <v>5.45</v>
       </c>
+      <c r="AC26" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -2982,8 +3071,11 @@
       <c r="AB27" s="1">
         <v>5.88</v>
       </c>
+      <c r="AC27" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -3068,8 +3160,11 @@
       <c r="AB28" s="1">
         <v>10.039999999999999</v>
       </c>
+      <c r="AC28" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -3154,8 +3249,11 @@
       <c r="AB29" s="1">
         <v>7.17</v>
       </c>
+      <c r="AC29" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -3240,8 +3338,11 @@
       <c r="AB30" s="1">
         <v>5.45</v>
       </c>
+      <c r="AC30" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -3326,8 +3427,11 @@
       <c r="AB31" s="1">
         <v>6.86</v>
       </c>
+      <c r="AC31" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -3412,8 +3516,11 @@
       <c r="AB32" s="1">
         <v>4.6100000000000003</v>
       </c>
+      <c r="AC32" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -3498,8 +3605,11 @@
       <c r="AB33" s="1">
         <v>6.9</v>
       </c>
+      <c r="AC33" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -3584,8 +3694,11 @@
       <c r="AB34" s="1">
         <v>5.78</v>
       </c>
+      <c r="AC34" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -3670,8 +3783,11 @@
       <c r="AB35" s="1">
         <v>5.93</v>
       </c>
+      <c r="AC35" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -3756,8 +3872,11 @@
       <c r="AB36" s="1">
         <v>10.050000000000001</v>
       </c>
+      <c r="AC36" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -3842,8 +3961,11 @@
       <c r="AB37" s="1">
         <v>4.84</v>
       </c>
+      <c r="AC37" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -3928,8 +4050,11 @@
       <c r="AB38" s="1">
         <v>6.43</v>
       </c>
+      <c r="AC38" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -4014,8 +4139,11 @@
       <c r="AB39" s="1">
         <v>7.9</v>
       </c>
+      <c r="AC39" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -4100,8 +4228,11 @@
       <c r="AB40" s="1">
         <v>5.04</v>
       </c>
+      <c r="AC40" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -4186,8 +4317,11 @@
       <c r="AB41" s="1">
         <v>5.04</v>
       </c>
+      <c r="AC41" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -4272,8 +4406,11 @@
       <c r="AB42" s="1">
         <v>5.28</v>
       </c>
+      <c r="AC42" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -4358,8 +4495,11 @@
       <c r="AB43" s="1">
         <v>10.01</v>
       </c>
+      <c r="AC43" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -4444,8 +4584,11 @@
       <c r="AB44" s="1">
         <v>6.89</v>
       </c>
+      <c r="AC44" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -4530,8 +4673,11 @@
       <c r="AB45" s="1">
         <v>6.97</v>
       </c>
+      <c r="AC45" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -4616,8 +4762,11 @@
       <c r="AB46" s="1">
         <v>4.82</v>
       </c>
+      <c r="AC46" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -4702,8 +4851,11 @@
       <c r="AB47" s="1">
         <v>9.49</v>
       </c>
+      <c r="AC47" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -4788,8 +4940,11 @@
       <c r="AB48" s="1">
         <v>4.96</v>
       </c>
+      <c r="AC48" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -4874,8 +5029,11 @@
       <c r="AB49" s="1">
         <v>6.08</v>
       </c>
+      <c r="AC49" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -4960,8 +5118,11 @@
       <c r="AB50" s="1">
         <v>4.37</v>
       </c>
+      <c r="AC50" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -5046,8 +5207,11 @@
       <c r="AB51" s="1">
         <v>5.24</v>
       </c>
+      <c r="AC51" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -5131,6 +5295,9 @@
       </c>
       <c r="AB52" s="1">
         <v>6.68</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mutual info code commented out at the end of data.ipynb
</commit_message>
<xml_diff>
--- a/states_correlation_dataset.xlsx
+++ b/states_correlation_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbcme\OneDrive\Documentos\GitHub\data-vis-nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BFEE7D-C7C3-4424-B3C7-DD97981A59E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31FBB0E-2384-459B-8308-E0C1F2730FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B280968C-2C0A-420C-A93E-E5F0EEDC2270}"/>
   </bookViews>
@@ -271,9 +271,6 @@
     <t>public_work</t>
   </si>
   <si>
-    <t>selfempoyed</t>
-  </si>
-  <si>
     <t>party_2020</t>
   </si>
   <si>
@@ -281,6 +278,9 @@
   </si>
   <si>
     <t>DEMOCRAT</t>
+  </si>
+  <si>
+    <t>selfemployed</t>
   </si>
 </sst>
 </file>
@@ -636,38 +636,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349CF4C0-C2B9-410F-AD99-9DA3A70DA3E4}">
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomLeft" activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.34765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.84765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.09765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.94921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.94921875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.1484375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.69921875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.94921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.796875" style="1" customWidth="1"/>
-    <col min="14" max="15" width="19.44921875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.44921875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6484375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.34765625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.59765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.296875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1484375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.44921875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.8984375" style="1" customWidth="1"/>
     <col min="23" max="23" width="13.25" style="1" customWidth="1"/>
-    <col min="24" max="24" width="22.19921875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6.8984375" style="1" customWidth="1"/>
-    <col min="26" max="28" width="8.796875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.44921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="16384" width="8.796875" style="1"/>
   </cols>
@@ -755,10 +758,10 @@
         <v>77</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.45">
@@ -847,7 +850,7 @@
         <v>5.18</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.45">
@@ -936,7 +939,7 @@
         <v>7.08</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.45">
@@ -1025,7 +1028,7 @@
         <v>6.39</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.45">
@@ -1114,7 +1117,7 @@
         <v>6.31</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.45">
@@ -1203,7 +1206,7 @@
         <v>8.48</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.45">
@@ -1292,7 +1295,7 @@
         <v>6.67</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.45">
@@ -1381,7 +1384,7 @@
         <v>6.37</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.45">
@@ -1470,7 +1473,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.45">
@@ -1559,7 +1562,7 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.45">
@@ -1648,7 +1651,7 @@
         <v>6.3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.45">
@@ -1737,7 +1740,7 @@
         <v>5.58</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.45">
@@ -1826,7 +1829,7 @@
         <v>7.27</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.45">
@@ -1915,7 +1918,7 @@
         <v>7.92</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.45">
@@ -2004,7 +2007,7 @@
         <v>4.74</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.45">
@@ -2093,7 +2096,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.45">
@@ -2182,7 +2185,7 @@
         <v>7.08</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.45">
@@ -2271,7 +2274,7 @@
         <v>6.66</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.45">
@@ -2360,7 +2363,7 @@
         <v>5.64</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.45">
@@ -2449,7 +2452,7 @@
         <v>5.78</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.45">
@@ -2538,7 +2541,7 @@
         <v>9.18</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.45">
@@ -2627,7 +2630,7 @@
         <v>4.88</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.45">
@@ -2716,7 +2719,7 @@
         <v>5.96</v>
       </c>
       <c r="AC23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.45">
@@ -2805,7 +2808,7 @@
         <v>5.04</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
@@ -2894,7 +2897,7 @@
         <v>5.88</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
@@ -2983,7 +2986,7 @@
         <v>5.45</v>
       </c>
       <c r="AC26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
@@ -3072,7 +3075,7 @@
         <v>5.88</v>
       </c>
       <c r="AC27" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
@@ -3161,7 +3164,7 @@
         <v>10.039999999999999</v>
       </c>
       <c r="AC28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
@@ -3250,7 +3253,7 @@
         <v>7.17</v>
       </c>
       <c r="AC29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
@@ -3339,7 +3342,7 @@
         <v>5.45</v>
       </c>
       <c r="AC30" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
@@ -3428,7 +3431,7 @@
         <v>6.86</v>
       </c>
       <c r="AC31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
@@ -3517,7 +3520,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="AC32" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.45">
@@ -3606,7 +3609,7 @@
         <v>6.9</v>
       </c>
       <c r="AC33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.45">
@@ -3695,7 +3698,7 @@
         <v>5.78</v>
       </c>
       <c r="AC34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.45">
@@ -3784,7 +3787,7 @@
         <v>5.93</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.45">
@@ -3873,7 +3876,7 @@
         <v>10.050000000000001</v>
       </c>
       <c r="AC36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.45">
@@ -3962,7 +3965,7 @@
         <v>4.84</v>
       </c>
       <c r="AC37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.45">
@@ -4051,7 +4054,7 @@
         <v>6.43</v>
       </c>
       <c r="AC38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.45">
@@ -4140,7 +4143,7 @@
         <v>7.9</v>
       </c>
       <c r="AC39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.45">
@@ -4229,7 +4232,7 @@
         <v>5.04</v>
       </c>
       <c r="AC40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.45">
@@ -4318,7 +4321,7 @@
         <v>5.04</v>
       </c>
       <c r="AC41" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.45">
@@ -4407,7 +4410,7 @@
         <v>5.28</v>
       </c>
       <c r="AC42" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.45">
@@ -4496,7 +4499,7 @@
         <v>10.01</v>
       </c>
       <c r="AC43" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.45">
@@ -4585,7 +4588,7 @@
         <v>6.89</v>
       </c>
       <c r="AC44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.45">
@@ -4674,7 +4677,7 @@
         <v>6.97</v>
       </c>
       <c r="AC45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.45">
@@ -4763,7 +4766,7 @@
         <v>4.82</v>
       </c>
       <c r="AC46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.45">
@@ -4852,7 +4855,7 @@
         <v>9.49</v>
       </c>
       <c r="AC47" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.45">
@@ -4941,7 +4944,7 @@
         <v>4.96</v>
       </c>
       <c r="AC48" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.45">
@@ -5030,7 +5033,7 @@
         <v>6.08</v>
       </c>
       <c r="AC49" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.45">
@@ -5119,7 +5122,7 @@
         <v>4.37</v>
       </c>
       <c r="AC50" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.45">
@@ -5208,7 +5211,7 @@
         <v>5.24</v>
       </c>
       <c r="AC51" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.45">
@@ -5297,7 +5300,7 @@
         <v>6.68</v>
       </c>
       <c r="AC52" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pot3, plot4, plot5
</commit_message>
<xml_diff>
--- a/states_correlation_dataset.xlsx
+++ b/states_correlation_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbcme\OneDrive\Documentos\GitHub\data-vis-nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CFA658-DA87-4A2A-9945-29E37A60C623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C402E2AF-D5B9-4ECE-9684-E18F76E9F919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10590" yWindow="-19935" windowWidth="17100" windowHeight="9945" xr2:uid="{B280968C-2C0A-420C-A93E-E5F0EEDC2270}"/>
+    <workbookView xWindow="8595" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{B280968C-2C0A-420C-A93E-E5F0EEDC2270}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="133">
   <si>
     <t>population</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Asian</t>
   </si>
   <si>
-    <t>Two or more races</t>
-  </si>
-  <si>
     <t>Foreign born</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
   </si>
   <si>
     <t>Self-employed</t>
-  </si>
-  <si>
-    <t>Pacific islander</t>
   </si>
   <si>
     <t>Unemployed</t>
@@ -446,6 +440,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,12 +471,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -796,11 +796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349CF4C0-C2B9-410F-AD99-9DA3A70DA3E4}">
-  <dimension ref="A1:AE52"/>
+  <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -817,40 +817,38 @@
     <col min="10" max="10" width="5.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.94921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.84765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.94921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.44921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.94921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.8984375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.94921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="8.796875" style="1"/>
+    <col min="13" max="13" width="10.94921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.84765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.94921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.44921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.94921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.8984375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.6484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.94921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>56</v>
@@ -877,46 +875,46 @@
         <v>63</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>70</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>76</v>
@@ -925,21 +923,15 @@
         <v>78</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1">
         <v>5024279</v>
@@ -973,69 +965,63 @@
         <v>1.5</v>
       </c>
       <c r="M2" s="1">
-        <v>0.1</v>
+        <v>3.4</v>
       </c>
       <c r="N2" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="O2" s="1">
-        <v>3.4</v>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="O2" s="3">
+        <v>49.12174439733495</v>
       </c>
       <c r="P2" s="1">
-        <v>2.5299999999999998</v>
+        <v>5.3</v>
       </c>
       <c r="Q2" s="1">
-        <v>811</v>
+        <v>87.9</v>
       </c>
       <c r="R2" s="1">
-        <v>5.3</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="S2" s="1">
-        <v>87.9</v>
+        <v>86.9</v>
       </c>
       <c r="T2" s="1">
-        <v>79.900000000000006</v>
+        <v>26.2</v>
       </c>
       <c r="U2" s="1">
-        <v>86.9</v>
+        <v>11.5</v>
       </c>
       <c r="V2" s="1">
-        <v>26.2</v>
+        <v>11.7</v>
       </c>
       <c r="W2" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="X2" s="1">
-        <v>11.7</v>
+        <v>25.2</v>
+      </c>
+      <c r="X2" s="3">
+        <v>57.280773210629441</v>
       </c>
       <c r="Y2" s="1">
-        <v>25.2</v>
+        <v>14.9</v>
       </c>
       <c r="Z2" s="1">
-        <v>52035</v>
+        <v>79.16</v>
       </c>
       <c r="AA2" s="1">
-        <v>14.9</v>
+        <v>15.46</v>
       </c>
       <c r="AB2" s="1">
-        <v>79.16</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>15.46</v>
-      </c>
-      <c r="AD2" s="1">
         <v>5.18</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" s="1">
         <v>733391</v>
@@ -1069,69 +1055,63 @@
         <v>6.5</v>
       </c>
       <c r="M3" s="1">
-        <v>1.4</v>
+        <v>7.8</v>
       </c>
       <c r="N3" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="O3" s="1">
-        <v>7.8</v>
+        <v>2.78</v>
+      </c>
+      <c r="O3" s="3">
+        <v>75.105996365838891</v>
       </c>
       <c r="P3" s="1">
-        <v>2.78</v>
+        <v>15.8</v>
       </c>
       <c r="Q3" s="1">
-        <v>1240</v>
+        <v>95</v>
       </c>
       <c r="R3" s="1">
-        <v>15.8</v>
+        <v>87.3</v>
       </c>
       <c r="S3" s="1">
-        <v>95</v>
+        <v>93.1</v>
       </c>
       <c r="T3" s="1">
-        <v>87.3</v>
+        <v>30</v>
       </c>
       <c r="U3" s="1">
-        <v>93.1</v>
+        <v>8.9</v>
       </c>
       <c r="V3" s="1">
-        <v>30</v>
+        <v>13.9</v>
       </c>
       <c r="W3" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="X3" s="1">
-        <v>13.9</v>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="X3" s="3">
+        <v>85.632196561062074</v>
       </c>
       <c r="Y3" s="1">
-        <v>18.899999999999999</v>
+        <v>9.6</v>
       </c>
       <c r="Z3" s="1">
-        <v>77790</v>
+        <v>65.23</v>
       </c>
       <c r="AA3" s="1">
-        <v>9.6</v>
+        <v>27.46</v>
       </c>
       <c r="AB3" s="1">
-        <v>65.23</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>27.46</v>
-      </c>
-      <c r="AD3" s="1">
         <v>7.08</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1">
         <v>7151502</v>
@@ -1165,69 +1145,63 @@
         <v>3.7</v>
       </c>
       <c r="M4" s="1">
-        <v>0.3</v>
+        <v>13.2</v>
       </c>
       <c r="N4" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="O4" s="1">
-        <v>13.2</v>
+        <v>2.65</v>
+      </c>
+      <c r="O4" s="3">
+        <v>66.444579043004239</v>
       </c>
       <c r="P4" s="1">
-        <v>2.65</v>
+        <v>26.7</v>
       </c>
       <c r="Q4" s="1">
-        <v>1097</v>
+        <v>93.3</v>
       </c>
       <c r="R4" s="1">
-        <v>26.7</v>
+        <v>86.6</v>
       </c>
       <c r="S4" s="1">
-        <v>93.3</v>
+        <v>87.9</v>
       </c>
       <c r="T4" s="1">
-        <v>86.6</v>
+        <v>30.3</v>
       </c>
       <c r="U4" s="1">
-        <v>87.9</v>
+        <v>8.9</v>
       </c>
       <c r="V4" s="1">
-        <v>30.3</v>
+        <v>13.6</v>
       </c>
       <c r="W4" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="X4" s="1">
-        <v>13.6</v>
+        <v>25.8</v>
+      </c>
+      <c r="X4" s="3">
+        <v>67.731886131965396</v>
       </c>
       <c r="Y4" s="1">
-        <v>25.8</v>
+        <v>12.8</v>
       </c>
       <c r="Z4" s="1">
-        <v>61529</v>
+        <v>78.78</v>
       </c>
       <c r="AA4" s="1">
-        <v>12.8</v>
+        <v>14.67</v>
       </c>
       <c r="AB4" s="1">
-        <v>78.78</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>14.67</v>
-      </c>
-      <c r="AD4" s="1">
         <v>6.39</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1">
         <v>3011524</v>
@@ -1261,69 +1235,63 @@
         <v>1.7</v>
       </c>
       <c r="M5" s="1">
-        <v>0.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N5" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O5" s="1">
-        <v>4.9000000000000004</v>
+        <v>2.5</v>
+      </c>
+      <c r="O5" s="3">
+        <v>46.032707450030287</v>
       </c>
       <c r="P5" s="1">
-        <v>2.5</v>
+        <v>7.6</v>
       </c>
       <c r="Q5" s="1">
-        <v>760</v>
+        <v>88.2</v>
       </c>
       <c r="R5" s="1">
-        <v>7.6</v>
+        <v>77</v>
       </c>
       <c r="S5" s="1">
-        <v>88.2</v>
+        <v>87.2</v>
       </c>
       <c r="T5" s="1">
-        <v>77</v>
+        <v>23.8</v>
       </c>
       <c r="U5" s="1">
-        <v>87.2</v>
+        <v>12.9</v>
       </c>
       <c r="V5" s="1">
-        <v>23.8</v>
+        <v>10.9</v>
       </c>
       <c r="W5" s="1">
-        <v>12.9</v>
-      </c>
-      <c r="X5" s="1">
-        <v>10.9</v>
+        <v>21.8</v>
+      </c>
+      <c r="X5" s="3">
+        <v>54.462693467779225</v>
       </c>
       <c r="Y5" s="1">
-        <v>21.8</v>
+        <v>15.2</v>
       </c>
       <c r="Z5" s="1">
-        <v>49475</v>
+        <v>77.16</v>
       </c>
       <c r="AA5" s="1">
-        <v>15.2</v>
+        <v>16.34</v>
       </c>
       <c r="AB5" s="1">
-        <v>77.16</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>16.34</v>
-      </c>
-      <c r="AD5" s="1">
         <v>6.31</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1">
         <v>39538223</v>
@@ -1357,69 +1325,63 @@
         <v>15.5</v>
       </c>
       <c r="M6" s="1">
-        <v>0.5</v>
+        <v>26.6</v>
       </c>
       <c r="N6" s="1">
-        <v>4</v>
-      </c>
-      <c r="O6" s="1">
-        <v>26.6</v>
+        <v>2.94</v>
+      </c>
+      <c r="O6" s="3">
+        <v>96.062992125984252</v>
       </c>
       <c r="P6" s="1">
-        <v>2.94</v>
+        <v>43.9</v>
       </c>
       <c r="Q6" s="1">
-        <v>1586</v>
+        <v>94.3</v>
       </c>
       <c r="R6" s="1">
-        <v>43.9</v>
+        <v>88.9</v>
       </c>
       <c r="S6" s="1">
-        <v>94.3</v>
+        <v>83.9</v>
       </c>
       <c r="T6" s="1">
-        <v>88.9</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="U6" s="1">
-        <v>83.9</v>
+        <v>6.8</v>
       </c>
       <c r="V6" s="1">
-        <v>34.700000000000003</v>
+        <v>8.9</v>
       </c>
       <c r="W6" s="1">
-        <v>6.8</v>
-      </c>
-      <c r="X6" s="1">
-        <v>8.9</v>
+        <v>29.8</v>
+      </c>
+      <c r="X6" s="3">
+        <v>86.603113097465936</v>
       </c>
       <c r="Y6" s="1">
-        <v>29.8</v>
+        <v>11.5</v>
       </c>
       <c r="Z6" s="1">
-        <v>78672</v>
+        <v>77.650000000000006</v>
       </c>
       <c r="AA6" s="1">
-        <v>11.5</v>
+        <v>13.69</v>
       </c>
       <c r="AB6" s="1">
-        <v>77.650000000000006</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>13.69</v>
-      </c>
-      <c r="AD6" s="1">
         <v>8.48</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1">
         <v>5773714</v>
@@ -1453,69 +1415,63 @@
         <v>3.5</v>
       </c>
       <c r="M7" s="1">
-        <v>0.2</v>
+        <v>9.5</v>
       </c>
       <c r="N7" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="O7" s="1">
-        <v>9.5</v>
+        <v>2.6</v>
+      </c>
+      <c r="O7" s="3">
+        <v>80.860084797092668</v>
       </c>
       <c r="P7" s="1">
-        <v>2.6</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="Q7" s="1">
-        <v>1335</v>
+        <v>94.9</v>
       </c>
       <c r="R7" s="1">
-        <v>16.399999999999999</v>
+        <v>89.6</v>
       </c>
       <c r="S7" s="1">
-        <v>94.9</v>
+        <v>92.1</v>
       </c>
       <c r="T7" s="1">
-        <v>89.6</v>
+        <v>41.6</v>
       </c>
       <c r="U7" s="1">
-        <v>92.1</v>
+        <v>7.4</v>
       </c>
       <c r="V7" s="1">
-        <v>41.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="W7" s="1">
-        <v>7.4</v>
-      </c>
-      <c r="X7" s="1">
-        <v>9.3000000000000007</v>
+        <v>24.8</v>
+      </c>
+      <c r="X7" s="3">
+        <v>82.815217630611386</v>
       </c>
       <c r="Y7" s="1">
-        <v>24.8</v>
+        <v>9</v>
       </c>
       <c r="Z7" s="1">
-        <v>75231</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="AA7" s="1">
-        <v>9</v>
+        <v>14.03</v>
       </c>
       <c r="AB7" s="1">
-        <v>79.099999999999994</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>14.03</v>
-      </c>
-      <c r="AD7" s="1">
         <v>6.67</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1">
         <v>3605944</v>
@@ -1549,69 +1505,63 @@
         <v>5</v>
       </c>
       <c r="M8" s="1">
-        <v>0.1</v>
+        <v>14.6</v>
       </c>
       <c r="N8" s="1">
         <v>2.5</v>
       </c>
-      <c r="O8" s="1">
-        <v>14.6</v>
+      <c r="O8" s="3">
+        <v>72.743791641429439</v>
       </c>
       <c r="P8" s="1">
-        <v>2.5</v>
+        <v>22.1</v>
       </c>
       <c r="Q8" s="1">
-        <v>1201</v>
+        <v>92</v>
       </c>
       <c r="R8" s="1">
-        <v>22.1</v>
+        <v>87.3</v>
       </c>
       <c r="S8" s="1">
-        <v>92</v>
+        <v>90.9</v>
       </c>
       <c r="T8" s="1">
-        <v>87.3</v>
+        <v>40</v>
       </c>
       <c r="U8" s="1">
-        <v>90.9</v>
+        <v>7.6</v>
       </c>
       <c r="V8" s="1">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="W8" s="1">
-        <v>7.6</v>
-      </c>
-      <c r="X8" s="1">
-        <v>7</v>
+        <v>26.7</v>
+      </c>
+      <c r="X8" s="3">
+        <v>87.905374166134607</v>
       </c>
       <c r="Y8" s="1">
-        <v>26.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="Z8" s="1">
-        <v>79855</v>
+        <v>80.709999999999994</v>
       </c>
       <c r="AA8" s="1">
-        <v>9.6999999999999993</v>
+        <v>12.73</v>
       </c>
       <c r="AB8" s="1">
-        <v>80.709999999999994</v>
-      </c>
-      <c r="AC8" s="1">
-        <v>12.73</v>
-      </c>
-      <c r="AD8" s="1">
         <v>6.37</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1">
         <v>689545</v>
@@ -1645,69 +1595,63 @@
         <v>4.5</v>
       </c>
       <c r="M9" s="1">
-        <v>0.1</v>
+        <v>13.4</v>
       </c>
       <c r="N9" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="O9" s="1">
-        <v>13.4</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O9" s="3">
+        <v>97.334948516050872</v>
       </c>
       <c r="P9" s="1">
-        <v>2.2999999999999998</v>
+        <v>17.2</v>
       </c>
       <c r="Q9" s="1">
-        <v>1607</v>
+        <v>93</v>
       </c>
       <c r="R9" s="1">
-        <v>17.2</v>
+        <v>85.6</v>
       </c>
       <c r="S9" s="1">
-        <v>93</v>
+        <v>91.9</v>
       </c>
       <c r="T9" s="1">
-        <v>85.6</v>
+        <v>59.8</v>
       </c>
       <c r="U9" s="1">
-        <v>91.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="V9" s="1">
-        <v>59.8</v>
+        <v>3.9</v>
       </c>
       <c r="W9" s="1">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="X9" s="1">
-        <v>3.9</v>
+        <v>30.9</v>
+      </c>
+      <c r="X9" s="3">
+        <v>100</v>
       </c>
       <c r="Y9" s="1">
-        <v>30.9</v>
+        <v>15</v>
       </c>
       <c r="Z9" s="1">
-        <v>90842</v>
+        <v>70.66</v>
       </c>
       <c r="AA9" s="1">
-        <v>15</v>
+        <v>25.11</v>
       </c>
       <c r="AB9" s="1">
-        <v>70.66</v>
-      </c>
-      <c r="AC9" s="1">
-        <v>25.11</v>
-      </c>
-      <c r="AD9" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1">
         <v>989948</v>
@@ -1741,69 +1685,63 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="M10" s="1">
-        <v>0.1</v>
+        <v>9.4</v>
       </c>
       <c r="N10" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="O10" s="1">
-        <v>9.4</v>
+        <v>2.54</v>
+      </c>
+      <c r="O10" s="3">
+        <v>69.654754694124776</v>
       </c>
       <c r="P10" s="1">
-        <v>2.54</v>
+        <v>13.4</v>
       </c>
       <c r="Q10" s="1">
-        <v>1150</v>
+        <v>93.1</v>
       </c>
       <c r="R10" s="1">
-        <v>13.4</v>
+        <v>87.4</v>
       </c>
       <c r="S10" s="1">
-        <v>93.1</v>
+        <v>90.6</v>
       </c>
       <c r="T10" s="1">
-        <v>87.4</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="U10" s="1">
-        <v>90.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="V10" s="1">
-        <v>32.700000000000003</v>
+        <v>8.1</v>
       </c>
       <c r="W10" s="1">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="X10" s="1">
-        <v>8.1</v>
+        <v>26.2</v>
+      </c>
+      <c r="X10" s="3">
+        <v>76.077144932960522</v>
       </c>
       <c r="Y10" s="1">
-        <v>26.2</v>
+        <v>10.9</v>
       </c>
       <c r="Z10" s="1">
-        <v>69110</v>
+        <v>81.709999999999994</v>
       </c>
       <c r="AA10" s="1">
-        <v>10.9</v>
+        <v>14.06</v>
       </c>
       <c r="AB10" s="1">
-        <v>81.709999999999994</v>
-      </c>
-      <c r="AC10" s="1">
-        <v>14.06</v>
-      </c>
-      <c r="AD10" s="1">
         <v>4.1100000000000003</v>
       </c>
-      <c r="AE10" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1">
         <v>21538187</v>
@@ -1837,69 +1775,63 @@
         <v>3</v>
       </c>
       <c r="M11" s="1">
-        <v>0.1</v>
+        <v>20.8</v>
       </c>
       <c r="N11" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O11" s="1">
-        <v>20.8</v>
+        <v>2.62</v>
+      </c>
+      <c r="O11" s="3">
+        <v>73.773470623864327</v>
       </c>
       <c r="P11" s="1">
-        <v>2.62</v>
+        <v>29.4</v>
       </c>
       <c r="Q11" s="1">
-        <v>1218</v>
+        <v>93.1</v>
       </c>
       <c r="R11" s="1">
-        <v>29.4</v>
+        <v>85.4</v>
       </c>
       <c r="S11" s="1">
-        <v>93.1</v>
+        <v>88.5</v>
       </c>
       <c r="T11" s="1">
-        <v>85.4</v>
+        <v>30.5</v>
       </c>
       <c r="U11" s="1">
-        <v>88.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="V11" s="1">
-        <v>30.5</v>
+        <v>16.3</v>
       </c>
       <c r="W11" s="1">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="X11" s="1">
-        <v>16.3</v>
+        <v>27.9</v>
+      </c>
+      <c r="X11" s="3">
+        <v>63.520177891283765</v>
       </c>
       <c r="Y11" s="1">
-        <v>27.9</v>
+        <v>12.4</v>
       </c>
       <c r="Z11" s="1">
-        <v>57703</v>
+        <v>81.5</v>
       </c>
       <c r="AA11" s="1">
-        <v>12.4</v>
+        <v>12.01</v>
       </c>
       <c r="AB11" s="1">
-        <v>81.5</v>
-      </c>
-      <c r="AC11" s="1">
-        <v>12.01</v>
-      </c>
-      <c r="AD11" s="1">
         <v>6.3</v>
       </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="1">
         <v>10711908</v>
@@ -1933,69 +1865,63 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="M12" s="1">
-        <v>0.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="N12" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O12" s="1">
-        <v>10.199999999999999</v>
+        <v>2.68</v>
+      </c>
+      <c r="O12" s="3">
+        <v>63.113264688067837</v>
       </c>
       <c r="P12" s="1">
-        <v>2.68</v>
+        <v>14</v>
       </c>
       <c r="Q12" s="1">
-        <v>1042</v>
+        <v>92</v>
       </c>
       <c r="R12" s="1">
+        <v>84.4</v>
+      </c>
+      <c r="S12" s="1">
+        <v>87.9</v>
+      </c>
+      <c r="T12" s="1">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="U12" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="V12" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="W12" s="1">
+        <v>28.7</v>
+      </c>
+      <c r="X12" s="3">
+        <v>67.396138350102376</v>
+      </c>
+      <c r="Y12" s="1">
         <v>14</v>
       </c>
-      <c r="S12" s="1">
-        <v>92</v>
-      </c>
-      <c r="T12" s="1">
-        <v>84.4</v>
-      </c>
-      <c r="U12" s="1">
-        <v>87.9</v>
-      </c>
-      <c r="V12" s="1">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="W12" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="X12" s="1">
-        <v>15.5</v>
-      </c>
-      <c r="Y12" s="1">
-        <v>28.7</v>
-      </c>
       <c r="Z12" s="1">
-        <v>61224</v>
+        <v>78.88</v>
       </c>
       <c r="AA12" s="1">
-        <v>14</v>
+        <v>15.38</v>
       </c>
       <c r="AB12" s="1">
-        <v>78.88</v>
-      </c>
-      <c r="AC12" s="1">
-        <v>15.38</v>
-      </c>
-      <c r="AD12" s="1">
         <v>5.58</v>
       </c>
-      <c r="AE12" s="1" t="s">
+      <c r="AC12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="1">
         <v>1455271</v>
@@ -2029,69 +1955,63 @@
         <v>37.6</v>
       </c>
       <c r="M13" s="1">
-        <v>10.1</v>
+        <v>18.3</v>
       </c>
       <c r="N13" s="1">
-        <v>24.2</v>
-      </c>
-      <c r="O13" s="1">
-        <v>18.3</v>
+        <v>2.94</v>
+      </c>
+      <c r="O13" s="3">
+        <v>100</v>
       </c>
       <c r="P13" s="1">
-        <v>2.94</v>
+        <v>26.1</v>
       </c>
       <c r="Q13" s="1">
-        <v>1651</v>
+        <v>92.7</v>
       </c>
       <c r="R13" s="1">
-        <v>26.1</v>
+        <v>87.1</v>
       </c>
       <c r="S13" s="1">
-        <v>92.7</v>
+        <v>92.5</v>
       </c>
       <c r="T13" s="1">
-        <v>87.1</v>
+        <v>33.6</v>
       </c>
       <c r="U13" s="1">
-        <v>92.5</v>
+        <v>6.4</v>
       </c>
       <c r="V13" s="1">
-        <v>33.6</v>
+        <v>5</v>
       </c>
       <c r="W13" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="X13" s="1">
-        <v>5</v>
+        <v>27.1</v>
+      </c>
+      <c r="X13" s="3">
+        <v>91.557869707844389</v>
       </c>
       <c r="Y13" s="1">
-        <v>27.1</v>
+        <v>8.9</v>
       </c>
       <c r="Z13" s="1">
-        <v>83173</v>
+        <v>70.650000000000006</v>
       </c>
       <c r="AA13" s="1">
-        <v>8.9</v>
+        <v>21.89</v>
       </c>
       <c r="AB13" s="1">
-        <v>70.650000000000006</v>
-      </c>
-      <c r="AC13" s="1">
-        <v>21.89</v>
-      </c>
-      <c r="AD13" s="1">
         <v>7.27</v>
       </c>
-      <c r="AE13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1">
         <v>1839106</v>
@@ -2125,69 +2045,63 @@
         <v>1.6</v>
       </c>
       <c r="M14" s="1">
-        <v>0.2</v>
+        <v>5.9</v>
       </c>
       <c r="N14" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="O14" s="1">
-        <v>5.9</v>
+        <v>2.66</v>
+      </c>
+      <c r="O14" s="3">
+        <v>53.725015142337973</v>
       </c>
       <c r="P14" s="1">
-        <v>2.66</v>
+        <v>10.8</v>
       </c>
       <c r="Q14" s="1">
-        <v>887</v>
+        <v>93.2</v>
       </c>
       <c r="R14" s="1">
-        <v>10.8</v>
+        <v>86</v>
       </c>
       <c r="S14" s="1">
-        <v>93.2</v>
+        <v>91.3</v>
       </c>
       <c r="T14" s="1">
-        <v>86</v>
+        <v>28.7</v>
       </c>
       <c r="U14" s="1">
-        <v>91.3</v>
+        <v>9.5</v>
       </c>
       <c r="V14" s="1">
         <v>28.7</v>
       </c>
       <c r="W14" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="X14" s="1">
-        <v>28.7</v>
+        <v>21.2</v>
+      </c>
+      <c r="X14" s="3">
+        <v>64.854362519539421</v>
       </c>
       <c r="Y14" s="1">
-        <v>21.2</v>
+        <v>10.1</v>
       </c>
       <c r="Z14" s="1">
-        <v>58915</v>
+        <v>75.91</v>
       </c>
       <c r="AA14" s="1">
-        <v>10.1</v>
+        <v>15.87</v>
       </c>
       <c r="AB14" s="1">
-        <v>75.91</v>
-      </c>
-      <c r="AC14" s="1">
-        <v>15.87</v>
-      </c>
-      <c r="AD14" s="1">
         <v>7.92</v>
       </c>
-      <c r="AE14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1">
         <v>12812508</v>
@@ -2221,69 +2135,63 @@
         <v>5.9</v>
       </c>
       <c r="M15" s="1">
-        <v>0.1</v>
+        <v>13.9</v>
       </c>
       <c r="N15" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="O15" s="1">
-        <v>13.9</v>
+        <v>2.54</v>
+      </c>
+      <c r="O15" s="3">
+        <v>62.870987280436097</v>
       </c>
       <c r="P15" s="1">
-        <v>2.54</v>
+        <v>23</v>
       </c>
       <c r="Q15" s="1">
-        <v>1038</v>
+        <v>91.5</v>
       </c>
       <c r="R15" s="1">
-        <v>23</v>
+        <v>85.4</v>
       </c>
       <c r="S15" s="1">
-        <v>91.5</v>
+        <v>89.7</v>
       </c>
       <c r="T15" s="1">
-        <v>85.4</v>
+        <v>35.5</v>
       </c>
       <c r="U15" s="1">
-        <v>89.7</v>
+        <v>7.3</v>
       </c>
       <c r="V15" s="1">
-        <v>35.5</v>
+        <v>8.6</v>
       </c>
       <c r="W15" s="1">
-        <v>7.3</v>
-      </c>
-      <c r="X15" s="1">
-        <v>8.6</v>
+        <v>29</v>
+      </c>
+      <c r="X15" s="3">
+        <v>75.326390876466832</v>
       </c>
       <c r="Y15" s="1">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="Z15" s="1">
-        <v>68428</v>
+        <v>82.71</v>
       </c>
       <c r="AA15" s="1">
-        <v>11</v>
+        <v>12.4</v>
       </c>
       <c r="AB15" s="1">
-        <v>82.71</v>
-      </c>
-      <c r="AC15" s="1">
-        <v>12.4</v>
-      </c>
-      <c r="AD15" s="1">
         <v>4.74</v>
       </c>
-      <c r="AE15" s="1" t="s">
+      <c r="AC15" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1">
         <v>6785528</v>
@@ -2317,69 +2225,63 @@
         <v>2.6</v>
       </c>
       <c r="M16" s="1">
-        <v>0.1</v>
+        <v>5.3</v>
       </c>
       <c r="N16" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O16" s="1">
-        <v>5.3</v>
+        <v>2.5</v>
+      </c>
+      <c r="O16" s="3">
+        <v>51.120533010296789</v>
       </c>
       <c r="P16" s="1">
-        <v>2.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="Q16" s="1">
-        <v>844</v>
+        <v>90.3</v>
       </c>
       <c r="R16" s="1">
-        <v>8.8000000000000007</v>
+        <v>83.2</v>
       </c>
       <c r="S16" s="1">
-        <v>90.3</v>
+        <v>89.3</v>
       </c>
       <c r="T16" s="1">
-        <v>83.2</v>
+        <v>27.2</v>
       </c>
       <c r="U16" s="1">
-        <v>89.3</v>
+        <v>9.9</v>
       </c>
       <c r="V16" s="1">
-        <v>27.2</v>
+        <v>10.3</v>
       </c>
       <c r="W16" s="1">
-        <v>9.9</v>
-      </c>
-      <c r="X16" s="1">
-        <v>10.3</v>
+        <v>23.9</v>
+      </c>
+      <c r="X16" s="3">
+        <v>64.10581008784483</v>
       </c>
       <c r="Y16" s="1">
-        <v>23.9</v>
+        <v>11.6</v>
       </c>
       <c r="Z16" s="1">
-        <v>58235</v>
+        <v>84.7</v>
       </c>
       <c r="AA16" s="1">
-        <v>11.6</v>
+        <v>10.5</v>
       </c>
       <c r="AB16" s="1">
-        <v>84.7</v>
-      </c>
-      <c r="AC16" s="1">
-        <v>10.5</v>
-      </c>
-      <c r="AD16" s="1">
         <v>4.6399999999999997</v>
       </c>
-      <c r="AE16" s="1" t="s">
+      <c r="AC16" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C17" s="1">
         <v>3190369</v>
@@ -2413,69 +2315,63 @@
         <v>2.7</v>
       </c>
       <c r="M17" s="1">
-        <v>0.2</v>
+        <v>5.4</v>
       </c>
       <c r="N17" s="1">
-        <v>2</v>
-      </c>
-      <c r="O17" s="1">
-        <v>5.4</v>
+        <v>2.4</v>
+      </c>
+      <c r="O17" s="3">
+        <v>48.818897637795274</v>
       </c>
       <c r="P17" s="1">
-        <v>2.4</v>
+        <v>8.4</v>
       </c>
       <c r="Q17" s="1">
-        <v>806</v>
+        <v>90.4</v>
       </c>
       <c r="R17" s="1">
-        <v>8.4</v>
+        <v>83.1</v>
       </c>
       <c r="S17" s="1">
-        <v>90.4</v>
+        <v>92.5</v>
       </c>
       <c r="T17" s="1">
-        <v>83.1</v>
+        <v>29.3</v>
       </c>
       <c r="U17" s="1">
-        <v>92.5</v>
+        <v>8</v>
       </c>
       <c r="V17" s="1">
-        <v>29.3</v>
+        <v>6</v>
       </c>
       <c r="W17" s="1">
-        <v>8</v>
-      </c>
-      <c r="X17" s="1">
-        <v>6</v>
+        <v>19.5</v>
+      </c>
+      <c r="X17" s="3">
+        <v>68.069835538627515</v>
       </c>
       <c r="Y17" s="1">
-        <v>19.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="Z17" s="1">
-        <v>61836</v>
+        <v>79.849999999999994</v>
       </c>
       <c r="AA17" s="1">
-        <v>10.199999999999999</v>
+        <v>12.85</v>
       </c>
       <c r="AB17" s="1">
-        <v>79.849999999999994</v>
-      </c>
-      <c r="AC17" s="1">
-        <v>12.85</v>
-      </c>
-      <c r="AD17" s="1">
         <v>7.08</v>
       </c>
-      <c r="AE17" s="1" t="s">
+      <c r="AC17" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C18" s="1">
         <v>2937880</v>
@@ -2509,69 +2405,63 @@
         <v>3.2</v>
       </c>
       <c r="M18" s="1">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="N18" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="O18" s="1">
-        <v>7</v>
+        <v>2.48</v>
+      </c>
+      <c r="O18" s="3">
+        <v>52.27135069654755</v>
       </c>
       <c r="P18" s="1">
-        <v>2.48</v>
+        <v>11.7</v>
       </c>
       <c r="Q18" s="1">
-        <v>863</v>
+        <v>91.7</v>
       </c>
       <c r="R18" s="1">
-        <v>11.7</v>
+        <v>84.5</v>
       </c>
       <c r="S18" s="1">
-        <v>91.7</v>
+        <v>91.4</v>
       </c>
       <c r="T18" s="1">
-        <v>84.5</v>
+        <v>33.9</v>
       </c>
       <c r="U18" s="1">
-        <v>91.4</v>
+        <v>9.1</v>
       </c>
       <c r="V18" s="1">
-        <v>33.9</v>
+        <v>10.9</v>
       </c>
       <c r="W18" s="1">
-        <v>9.1</v>
-      </c>
-      <c r="X18" s="1">
-        <v>10.9</v>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="X18" s="3">
+        <v>67.249730300962113</v>
       </c>
       <c r="Y18" s="1">
-        <v>19.600000000000001</v>
+        <v>10.6</v>
       </c>
       <c r="Z18" s="1">
-        <v>61091</v>
+        <v>77.739999999999995</v>
       </c>
       <c r="AA18" s="1">
-        <v>10.6</v>
+        <v>15.38</v>
       </c>
       <c r="AB18" s="1">
-        <v>77.739999999999995</v>
-      </c>
-      <c r="AC18" s="1">
-        <v>15.38</v>
-      </c>
-      <c r="AD18" s="1">
         <v>6.66</v>
       </c>
-      <c r="AE18" s="1" t="s">
+      <c r="AC18" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="1">
         <v>4505836</v>
@@ -2605,69 +2495,63 @@
         <v>1.6</v>
       </c>
       <c r="M19" s="1">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="N19" s="1">
-        <v>2</v>
-      </c>
-      <c r="O19" s="1">
-        <v>4</v>
+        <v>2.48</v>
+      </c>
+      <c r="O19" s="3">
+        <v>47.425802543912781</v>
       </c>
       <c r="P19" s="1">
-        <v>2.48</v>
+        <v>5.7</v>
       </c>
       <c r="Q19" s="1">
-        <v>783</v>
+        <v>88.5</v>
       </c>
       <c r="R19" s="1">
-        <v>5.7</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="S19" s="1">
-        <v>88.5</v>
+        <v>87.2</v>
       </c>
       <c r="T19" s="1">
-        <v>81.599999999999994</v>
+        <v>25</v>
       </c>
       <c r="U19" s="1">
-        <v>87.2</v>
+        <v>13.2</v>
       </c>
       <c r="V19" s="1">
-        <v>25</v>
+        <v>7.7</v>
       </c>
       <c r="W19" s="1">
-        <v>13.2</v>
-      </c>
-      <c r="X19" s="1">
-        <v>7.7</v>
+        <v>23.7</v>
+      </c>
+      <c r="X19" s="3">
+        <v>57.504238127738269</v>
       </c>
       <c r="Y19" s="1">
-        <v>23.7</v>
+        <v>14.9</v>
       </c>
       <c r="Z19" s="1">
-        <v>52238</v>
+        <v>79.27</v>
       </c>
       <c r="AA19" s="1">
         <v>14.9</v>
       </c>
       <c r="AB19" s="1">
-        <v>79.27</v>
-      </c>
-      <c r="AC19" s="1">
-        <v>14.9</v>
-      </c>
-      <c r="AD19" s="1">
         <v>5.64</v>
       </c>
-      <c r="AE19" s="1" t="s">
+      <c r="AC19" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="1">
         <v>4657757</v>
@@ -2701,69 +2585,63 @@
         <v>1.8</v>
       </c>
       <c r="M20" s="1">
-        <v>0.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="N20" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="O20" s="1">
-        <v>4.0999999999999996</v>
+        <v>2.59</v>
+      </c>
+      <c r="O20" s="3">
+        <v>53.058752271350698</v>
       </c>
       <c r="P20" s="1">
-        <v>2.59</v>
+        <v>7.8</v>
       </c>
       <c r="Q20" s="1">
-        <v>876</v>
+        <v>88.1</v>
       </c>
       <c r="R20" s="1">
-        <v>7.8</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="S20" s="1">
-        <v>88.1</v>
+        <v>85.9</v>
       </c>
       <c r="T20" s="1">
-        <v>79.099999999999994</v>
+        <v>24.9</v>
       </c>
       <c r="U20" s="1">
-        <v>85.9</v>
+        <v>11.2</v>
       </c>
       <c r="V20" s="1">
-        <v>24.9</v>
+        <v>10.5</v>
       </c>
       <c r="W20" s="1">
-        <v>11.2</v>
-      </c>
-      <c r="X20" s="1">
-        <v>10.5</v>
+        <v>25.8</v>
+      </c>
+      <c r="X20" s="3">
+        <v>55.921269897184125</v>
       </c>
       <c r="Y20" s="1">
-        <v>25.8</v>
+        <v>17.8</v>
       </c>
       <c r="Z20" s="1">
-        <v>50800</v>
+        <v>78.98</v>
       </c>
       <c r="AA20" s="1">
-        <v>17.8</v>
+        <v>15.1</v>
       </c>
       <c r="AB20" s="1">
-        <v>78.98</v>
-      </c>
-      <c r="AC20" s="1">
-        <v>15.1</v>
-      </c>
-      <c r="AD20" s="1">
         <v>5.78</v>
       </c>
-      <c r="AE20" s="1" t="s">
+      <c r="AC20" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1">
         <v>1362359</v>
@@ -2797,69 +2675,63 @@
         <v>1.3</v>
       </c>
       <c r="M21" s="1">
-        <v>0.1</v>
+        <v>3.6</v>
       </c>
       <c r="N21" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="O21" s="1">
-        <v>3.6</v>
+        <v>2.29</v>
+      </c>
+      <c r="O21" s="3">
+        <v>52.877044215626889</v>
       </c>
       <c r="P21" s="1">
-        <v>2.29</v>
+        <v>6</v>
       </c>
       <c r="Q21" s="1">
-        <v>873</v>
+        <v>91.1</v>
       </c>
       <c r="R21" s="1">
-        <v>6</v>
+        <v>84.3</v>
       </c>
       <c r="S21" s="1">
-        <v>91.1</v>
+        <v>93.2</v>
       </c>
       <c r="T21" s="1">
-        <v>84.3</v>
+        <v>32.5</v>
       </c>
       <c r="U21" s="1">
-        <v>93.2</v>
+        <v>11.5</v>
       </c>
       <c r="V21" s="1">
-        <v>32.5</v>
+        <v>10.1</v>
       </c>
       <c r="W21" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="X21" s="1">
-        <v>10.1</v>
+        <v>24.3</v>
+      </c>
+      <c r="X21" s="3">
+        <v>65.486228836881622</v>
       </c>
       <c r="Y21" s="1">
-        <v>24.3</v>
+        <v>10.6</v>
       </c>
       <c r="Z21" s="1">
-        <v>59489</v>
+        <v>76.75</v>
       </c>
       <c r="AA21" s="1">
-        <v>10.6</v>
+        <v>13.94</v>
       </c>
       <c r="AB21" s="1">
-        <v>76.75</v>
-      </c>
-      <c r="AC21" s="1">
-        <v>13.94</v>
-      </c>
-      <c r="AD21" s="1">
         <v>9.18</v>
       </c>
-      <c r="AE21" s="1" t="s">
+      <c r="AC21" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C22" s="1">
         <v>6177224</v>
@@ -2893,69 +2765,63 @@
         <v>6.7</v>
       </c>
       <c r="M22" s="1">
-        <v>0.1</v>
+        <v>15.2</v>
       </c>
       <c r="N22" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="O22" s="1">
-        <v>15.2</v>
+        <v>2.64</v>
+      </c>
+      <c r="O22" s="3">
+        <v>85.705632949727445</v>
       </c>
       <c r="P22" s="1">
-        <v>2.64</v>
+        <v>19</v>
       </c>
       <c r="Q22" s="1">
-        <v>1415</v>
+        <v>93.6</v>
       </c>
       <c r="R22" s="1">
-        <v>19</v>
+        <v>88.5</v>
       </c>
       <c r="S22" s="1">
-        <v>93.6</v>
+        <v>90.6</v>
       </c>
       <c r="T22" s="1">
-        <v>88.5</v>
+        <v>40.9</v>
       </c>
       <c r="U22" s="1">
-        <v>90.6</v>
+        <v>7.6</v>
       </c>
       <c r="V22" s="1">
-        <v>40.9</v>
+        <v>6.9</v>
       </c>
       <c r="W22" s="1">
-        <v>7.6</v>
-      </c>
-      <c r="X22" s="1">
-        <v>6.9</v>
+        <v>33</v>
+      </c>
+      <c r="X22" s="3">
+        <v>95.840029942097274</v>
       </c>
       <c r="Y22" s="1">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="Z22" s="1">
-        <v>87063</v>
+        <v>73.540000000000006</v>
       </c>
       <c r="AA22" s="1">
-        <v>9</v>
+        <v>21.47</v>
       </c>
       <c r="AB22" s="1">
-        <v>73.540000000000006</v>
-      </c>
-      <c r="AC22" s="1">
-        <v>21.47</v>
-      </c>
-      <c r="AD22" s="1">
         <v>4.88</v>
       </c>
-      <c r="AE22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="1">
         <v>7029917</v>
@@ -2989,69 +2855,63 @@
         <v>7.2</v>
       </c>
       <c r="M23" s="1">
-        <v>0.1</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="N23" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="O23" s="1">
-        <v>16.899999999999999</v>
+        <v>2.5</v>
+      </c>
+      <c r="O23" s="3">
+        <v>80.920654149000597</v>
       </c>
       <c r="P23" s="1">
-        <v>2.5</v>
+        <v>23.9</v>
       </c>
       <c r="Q23" s="1">
-        <v>1336</v>
+        <v>92.6</v>
       </c>
       <c r="R23" s="1">
-        <v>23.9</v>
+        <v>88.2</v>
       </c>
       <c r="S23" s="1">
-        <v>92.6</v>
+        <v>91.1</v>
       </c>
       <c r="T23" s="1">
-        <v>88.2</v>
+        <v>44.5</v>
       </c>
       <c r="U23" s="1">
-        <v>91.1</v>
+        <v>7.9</v>
       </c>
       <c r="V23" s="1">
-        <v>44.5</v>
+        <v>3.5</v>
       </c>
       <c r="W23" s="1">
-        <v>7.9</v>
-      </c>
-      <c r="X23" s="1">
-        <v>3.5</v>
+        <v>30</v>
+      </c>
+      <c r="X23" s="3">
+        <v>92.892054336100045</v>
       </c>
       <c r="Y23" s="1">
-        <v>30</v>
+        <v>9.4</v>
       </c>
       <c r="Z23" s="1">
-        <v>84385</v>
+        <v>81.86</v>
       </c>
       <c r="AA23" s="1">
-        <v>9.4</v>
+        <v>12.05</v>
       </c>
       <c r="AB23" s="1">
-        <v>81.86</v>
-      </c>
-      <c r="AC23" s="1">
-        <v>12.05</v>
-      </c>
-      <c r="AD23" s="1">
         <v>5.96</v>
       </c>
-      <c r="AE23" s="1" t="s">
+      <c r="AC23" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24" s="1">
         <v>10077331</v>
@@ -3085,69 +2945,63 @@
         <v>3.4</v>
       </c>
       <c r="M24" s="1">
-        <v>0.1</v>
+        <v>6.9</v>
       </c>
       <c r="N24" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="O24" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="O24" s="3">
+        <v>54.02786190187765</v>
+      </c>
+      <c r="P24" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>91.1</v>
+      </c>
+      <c r="R24" s="1">
+        <v>84.4</v>
+      </c>
+      <c r="S24" s="1">
+        <v>91.3</v>
+      </c>
+      <c r="T24" s="1">
+        <v>30</v>
+      </c>
+      <c r="U24" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="V24" s="1">
         <v>6.9</v>
       </c>
-      <c r="P24" s="1">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>892</v>
-      </c>
-      <c r="R24" s="1">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="S24" s="1">
-        <v>91.1</v>
-      </c>
-      <c r="T24" s="1">
-        <v>84.4</v>
-      </c>
-      <c r="U24" s="1">
-        <v>91.3</v>
-      </c>
-      <c r="V24" s="1">
-        <v>30</v>
-      </c>
       <c r="W24" s="1">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="X24" s="1">
-        <v>6.9</v>
+        <v>24.6</v>
+      </c>
+      <c r="X24" s="3">
+        <v>65.205521674996149</v>
       </c>
       <c r="Y24" s="1">
-        <v>24.6</v>
+        <v>12.6</v>
       </c>
       <c r="Z24" s="1">
-        <v>59234</v>
+        <v>84.18</v>
       </c>
       <c r="AA24" s="1">
-        <v>12.6</v>
+        <v>10.61</v>
       </c>
       <c r="AB24" s="1">
-        <v>84.18</v>
-      </c>
-      <c r="AC24" s="1">
-        <v>10.61</v>
-      </c>
-      <c r="AD24" s="1">
         <v>5.04</v>
       </c>
-      <c r="AE24" s="1" t="s">
+      <c r="AC24" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1">
         <v>5706494</v>
@@ -3181,69 +3035,63 @@
         <v>5.2</v>
       </c>
       <c r="M25" s="1">
-        <v>0.1</v>
+        <v>8.4</v>
       </c>
       <c r="N25" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="O25" s="1">
-        <v>8.4</v>
+        <v>2.48</v>
+      </c>
+      <c r="O25" s="3">
+        <v>61.175045427013927</v>
       </c>
       <c r="P25" s="1">
-        <v>2.48</v>
+        <v>11.9</v>
       </c>
       <c r="Q25" s="1">
-        <v>1010</v>
+        <v>92.7</v>
       </c>
       <c r="R25" s="1">
+        <v>87</v>
+      </c>
+      <c r="S25" s="1">
+        <v>93.4</v>
+      </c>
+      <c r="T25" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="U25" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="V25" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="W25" s="1">
+        <v>23.8</v>
+      </c>
+      <c r="X25" s="3">
+        <v>80.779815503841832</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>82.07</v>
+      </c>
+      <c r="AA25" s="1">
         <v>11.9</v>
       </c>
-      <c r="S25" s="1">
-        <v>92.7</v>
-      </c>
-      <c r="T25" s="1">
-        <v>87</v>
-      </c>
-      <c r="U25" s="1">
-        <v>93.4</v>
-      </c>
-      <c r="V25" s="1">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="W25" s="1">
-        <v>7.4</v>
-      </c>
-      <c r="X25" s="1">
-        <v>5.8</v>
-      </c>
-      <c r="Y25" s="1">
-        <v>23.8</v>
-      </c>
-      <c r="Z25" s="1">
-        <v>73382</v>
-      </c>
-      <c r="AA25" s="1">
-        <v>8.3000000000000007</v>
-      </c>
       <c r="AB25" s="1">
-        <v>82.07</v>
-      </c>
-      <c r="AC25" s="1">
-        <v>11.9</v>
-      </c>
-      <c r="AD25" s="1">
         <v>5.88</v>
       </c>
-      <c r="AE25" s="1" t="s">
+      <c r="AC25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" s="1">
         <v>2961279</v>
@@ -3277,69 +3125,63 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M26" s="1">
-        <v>0.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N26" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="O26" s="1">
-        <v>2.2999999999999998</v>
+        <v>2.59</v>
+      </c>
+      <c r="O26" s="3">
+        <v>47.789218655360386</v>
       </c>
       <c r="P26" s="1">
-        <v>2.59</v>
+        <v>4</v>
       </c>
       <c r="Q26" s="1">
-        <v>789</v>
+        <v>86.5</v>
       </c>
       <c r="R26" s="1">
-        <v>4</v>
+        <v>75.8</v>
       </c>
       <c r="S26" s="1">
-        <v>86.5</v>
+        <v>85.3</v>
       </c>
       <c r="T26" s="1">
-        <v>75.8</v>
+        <v>22.8</v>
       </c>
       <c r="U26" s="1">
-        <v>85.3</v>
+        <v>11.9</v>
       </c>
       <c r="V26" s="1">
-        <v>22.8</v>
+        <v>15.4</v>
       </c>
       <c r="W26" s="1">
-        <v>11.9</v>
-      </c>
-      <c r="X26" s="1">
-        <v>15.4</v>
+        <v>25.2</v>
+      </c>
+      <c r="X26" s="3">
+        <v>51.199885515510445</v>
       </c>
       <c r="Y26" s="1">
-        <v>25.2</v>
+        <v>18.7</v>
       </c>
       <c r="Z26" s="1">
-        <v>46511</v>
+        <v>75.91</v>
       </c>
       <c r="AA26" s="1">
-        <v>18.7</v>
+        <v>18.47</v>
       </c>
       <c r="AB26" s="1">
-        <v>75.91</v>
-      </c>
-      <c r="AC26" s="1">
-        <v>18.47</v>
-      </c>
-      <c r="AD26" s="1">
         <v>5.45</v>
       </c>
-      <c r="AE26" s="1" t="s">
+      <c r="AC26" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1">
         <v>6154913</v>
@@ -3373,69 +3215,63 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="M27" s="1">
-        <v>0.2</v>
+        <v>4.2</v>
       </c>
       <c r="N27" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="O27" s="1">
-        <v>4.2</v>
+        <v>2.44</v>
+      </c>
+      <c r="O27" s="3">
+        <v>51.059963658388853</v>
       </c>
       <c r="P27" s="1">
-        <v>2.44</v>
+        <v>6.3</v>
       </c>
       <c r="Q27" s="1">
-        <v>843</v>
+        <v>90.7</v>
       </c>
       <c r="R27" s="1">
-        <v>6.3</v>
+        <v>83.2</v>
       </c>
       <c r="S27" s="1">
-        <v>90.7</v>
+        <v>90.6</v>
       </c>
       <c r="T27" s="1">
-        <v>83.2</v>
+        <v>29.9</v>
       </c>
       <c r="U27" s="1">
-        <v>90.6</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="V27" s="1">
-        <v>29.9</v>
+        <v>12</v>
       </c>
       <c r="W27" s="1">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="X27" s="1">
-        <v>12</v>
+        <v>23.9</v>
+      </c>
+      <c r="X27" s="3">
+        <v>63.065542370269256</v>
       </c>
       <c r="Y27" s="1">
-        <v>23.9</v>
+        <v>12.1</v>
       </c>
       <c r="Z27" s="1">
-        <v>57290</v>
+        <v>81.5</v>
       </c>
       <c r="AA27" s="1">
-        <v>12.1</v>
+        <v>12.42</v>
       </c>
       <c r="AB27" s="1">
-        <v>81.5</v>
-      </c>
-      <c r="AC27" s="1">
-        <v>12.42</v>
-      </c>
-      <c r="AD27" s="1">
         <v>5.88</v>
       </c>
-      <c r="AE27" s="1" t="s">
+      <c r="AC27" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C28" s="1">
         <v>1084225</v>
@@ -3469,69 +3305,63 @@
         <v>0.9</v>
       </c>
       <c r="M28" s="1">
-        <v>0.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N28" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="O28" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.37</v>
+      </c>
+      <c r="O28" s="3">
+        <v>50.635978195033317</v>
       </c>
       <c r="P28" s="1">
-        <v>2.37</v>
+        <v>4</v>
       </c>
       <c r="Q28" s="1">
-        <v>836</v>
+        <v>90.5</v>
       </c>
       <c r="R28" s="1">
-        <v>4</v>
+        <v>83.3</v>
       </c>
       <c r="S28" s="1">
-        <v>90.5</v>
+        <v>94</v>
       </c>
       <c r="T28" s="1">
-        <v>83.3</v>
+        <v>33.1</v>
       </c>
       <c r="U28" s="1">
-        <v>94</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="V28" s="1">
-        <v>33.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="W28" s="1">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="X28" s="1">
-        <v>10.199999999999999</v>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="X28" s="3">
+        <v>62.238832258206557</v>
       </c>
       <c r="Y28" s="1">
-        <v>18.399999999999999</v>
+        <v>12.4</v>
       </c>
       <c r="Z28" s="1">
-        <v>56539</v>
+        <v>70.36</v>
       </c>
       <c r="AA28" s="1">
-        <v>12.4</v>
+        <v>19.04</v>
       </c>
       <c r="AB28" s="1">
-        <v>70.36</v>
-      </c>
-      <c r="AC28" s="1">
-        <v>19.04</v>
-      </c>
-      <c r="AD28" s="1">
         <v>10.039999999999999</v>
       </c>
-      <c r="AE28" s="1" t="s">
+      <c r="AC28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C29" s="1">
         <v>1961504</v>
@@ -3565,69 +3395,63 @@
         <v>2.7</v>
       </c>
       <c r="M29" s="1">
-        <v>0.1</v>
+        <v>7.4</v>
       </c>
       <c r="N29" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O29" s="1">
-        <v>7.4</v>
+        <v>2.44</v>
+      </c>
+      <c r="O29" s="3">
+        <v>51.907934585099937</v>
       </c>
       <c r="P29" s="1">
-        <v>2.44</v>
+        <v>11.8</v>
       </c>
       <c r="Q29" s="1">
-        <v>857</v>
+        <v>91.5</v>
       </c>
       <c r="R29" s="1">
-        <v>11.8</v>
+        <v>85.6</v>
       </c>
       <c r="S29" s="1">
-        <v>91.5</v>
+        <v>91.6</v>
       </c>
       <c r="T29" s="1">
-        <v>85.6</v>
+        <v>32.5</v>
       </c>
       <c r="U29" s="1">
-        <v>91.6</v>
+        <v>7.7</v>
       </c>
       <c r="V29" s="1">
-        <v>32.5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="W29" s="1">
-        <v>7.7</v>
-      </c>
-      <c r="X29" s="1">
-        <v>9.8000000000000007</v>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="X29" s="3">
+        <v>69.367693357697974</v>
       </c>
       <c r="Y29" s="1">
-        <v>18.899999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="Z29" s="1">
-        <v>63015</v>
+        <v>78.8</v>
       </c>
       <c r="AA29" s="1">
-        <v>9.1999999999999993</v>
+        <v>13.81</v>
       </c>
       <c r="AB29" s="1">
-        <v>78.8</v>
-      </c>
-      <c r="AC29" s="1">
-        <v>13.81</v>
-      </c>
-      <c r="AD29" s="1">
         <v>7.17</v>
       </c>
-      <c r="AE29" s="1" t="s">
+      <c r="AC29" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C30" s="1">
         <v>3104614</v>
@@ -3661,69 +3485,63 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="M30" s="1">
-        <v>0.8</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="N30" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="O30" s="1">
-        <v>19.399999999999999</v>
+        <v>2.65</v>
+      </c>
+      <c r="O30" s="3">
+        <v>70.199878861296185</v>
       </c>
       <c r="P30" s="1">
-        <v>2.65</v>
+        <v>30.2</v>
       </c>
       <c r="Q30" s="1">
-        <v>1159</v>
+        <v>93.6</v>
       </c>
       <c r="R30" s="1">
-        <v>30.2</v>
+        <v>85.5</v>
       </c>
       <c r="S30" s="1">
-        <v>93.6</v>
+        <v>86.9</v>
       </c>
       <c r="T30" s="1">
-        <v>85.5</v>
+        <v>25.5</v>
       </c>
       <c r="U30" s="1">
-        <v>86.9</v>
+        <v>8.5</v>
       </c>
       <c r="V30" s="1">
-        <v>25.5</v>
+        <v>13.4</v>
       </c>
       <c r="W30" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="X30" s="1">
-        <v>13.4</v>
+        <v>24.6</v>
+      </c>
+      <c r="X30" s="3">
+        <v>68.297703705334527</v>
       </c>
       <c r="Y30" s="1">
-        <v>24.6</v>
+        <v>12.5</v>
       </c>
       <c r="Z30" s="1">
-        <v>62043</v>
+        <v>82.33</v>
       </c>
       <c r="AA30" s="1">
-        <v>12.5</v>
+        <v>12.09</v>
       </c>
       <c r="AB30" s="1">
-        <v>82.33</v>
-      </c>
-      <c r="AC30" s="1">
-        <v>12.09</v>
-      </c>
-      <c r="AD30" s="1">
         <v>5.45</v>
       </c>
-      <c r="AE30" s="1" t="s">
+      <c r="AC30" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C31" s="1">
         <v>1377529</v>
@@ -3757,69 +3575,63 @@
         <v>3</v>
       </c>
       <c r="M31" s="1">
-        <v>0.1</v>
+        <v>6.1</v>
       </c>
       <c r="N31" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="O31" s="1">
-        <v>6.1</v>
+        <v>2.44</v>
+      </c>
+      <c r="O31" s="3">
+        <v>69.3519079345851</v>
       </c>
       <c r="P31" s="1">
-        <v>2.44</v>
+        <v>8.1</v>
       </c>
       <c r="Q31" s="1">
-        <v>1145</v>
+        <v>93.7</v>
       </c>
       <c r="R31" s="1">
-        <v>8.1</v>
+        <v>88.8</v>
       </c>
       <c r="S31" s="1">
-        <v>93.7</v>
+        <v>93.3</v>
       </c>
       <c r="T31" s="1">
-        <v>88.8</v>
+        <v>37.6</v>
       </c>
       <c r="U31" s="1">
-        <v>93.3</v>
+        <v>8.9</v>
       </c>
       <c r="V31" s="1">
-        <v>37.6</v>
+        <v>7.6</v>
       </c>
       <c r="W31" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="X31" s="1">
-        <v>7.6</v>
+        <v>27.4</v>
+      </c>
+      <c r="X31" s="3">
+        <v>85.778604610202322</v>
       </c>
       <c r="Y31" s="1">
-        <v>27.4</v>
+        <v>7</v>
       </c>
       <c r="Z31" s="1">
-        <v>77923</v>
+        <v>79.72</v>
       </c>
       <c r="AA31" s="1">
-        <v>7</v>
+        <v>13.29</v>
       </c>
       <c r="AB31" s="1">
-        <v>79.72</v>
-      </c>
-      <c r="AC31" s="1">
-        <v>13.29</v>
-      </c>
-      <c r="AD31" s="1">
         <v>6.86</v>
       </c>
-      <c r="AE31" s="1" t="s">
+      <c r="AC31" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C32" s="1">
         <v>9288994</v>
@@ -3853,69 +3665,63 @@
         <v>10</v>
       </c>
       <c r="M32" s="1">
-        <v>0.1</v>
+        <v>22.7</v>
       </c>
       <c r="N32" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O32" s="1">
-        <v>22.7</v>
+        <v>2.66</v>
+      </c>
+      <c r="O32" s="3">
+        <v>82.858873410054514</v>
       </c>
       <c r="P32" s="1">
-        <v>2.66</v>
+        <v>31.6</v>
       </c>
       <c r="Q32" s="1">
-        <v>1368</v>
+        <v>92.9</v>
       </c>
       <c r="R32" s="1">
-        <v>31.6</v>
+        <v>87.9</v>
       </c>
       <c r="S32" s="1">
-        <v>92.9</v>
+        <v>90.3</v>
       </c>
       <c r="T32" s="1">
-        <v>87.9</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="U32" s="1">
-        <v>90.3</v>
+        <v>6.6</v>
       </c>
       <c r="V32" s="1">
-        <v>40.700000000000003</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="W32" s="1">
-        <v>6.6</v>
-      </c>
-      <c r="X32" s="1">
-        <v>9.1999999999999993</v>
+        <v>32</v>
+      </c>
+      <c r="X32" s="3">
+        <v>93.83875299971379</v>
       </c>
       <c r="Y32" s="1">
-        <v>32</v>
+        <v>9.4</v>
       </c>
       <c r="Z32" s="1">
-        <v>85245</v>
+        <v>81.56</v>
       </c>
       <c r="AA32" s="1">
-        <v>9.4</v>
+        <v>13.68</v>
       </c>
       <c r="AB32" s="1">
-        <v>81.56</v>
-      </c>
-      <c r="AC32" s="1">
-        <v>13.68</v>
-      </c>
-      <c r="AD32" s="1">
         <v>4.6100000000000003</v>
       </c>
-      <c r="AE32" s="1" t="s">
+      <c r="AC32" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C33" s="1">
         <v>2117522</v>
@@ -3949,69 +3755,63 @@
         <v>1.8</v>
       </c>
       <c r="M33" s="1">
-        <v>0.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="N33" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="O33" s="1">
-        <v>9.1999999999999993</v>
+        <v>2.59</v>
+      </c>
+      <c r="O33" s="3">
+        <v>51.907934585099937</v>
       </c>
       <c r="P33" s="1">
-        <v>2.59</v>
+        <v>33.5</v>
       </c>
       <c r="Q33" s="1">
-        <v>857</v>
+        <v>88.1</v>
       </c>
       <c r="R33" s="1">
-        <v>33.5</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="S33" s="1">
-        <v>88.1</v>
+        <v>86.5</v>
       </c>
       <c r="T33" s="1">
-        <v>77.900000000000006</v>
+        <v>28.1</v>
       </c>
       <c r="U33" s="1">
-        <v>86.5</v>
+        <v>10.9</v>
       </c>
       <c r="V33" s="1">
-        <v>28.1</v>
+        <v>12</v>
       </c>
       <c r="W33" s="1">
-        <v>10.9</v>
-      </c>
-      <c r="X33" s="1">
-        <v>12</v>
+        <v>22.7</v>
+      </c>
+      <c r="X33" s="3">
+        <v>56.408929790185155</v>
       </c>
       <c r="Y33" s="1">
-        <v>22.7</v>
+        <v>16.8</v>
       </c>
       <c r="Z33" s="1">
-        <v>51243</v>
+        <v>69.63</v>
       </c>
       <c r="AA33" s="1">
-        <v>16.8</v>
+        <v>23.36</v>
       </c>
       <c r="AB33" s="1">
-        <v>69.63</v>
-      </c>
-      <c r="AC33" s="1">
-        <v>23.36</v>
-      </c>
-      <c r="AD33" s="1">
         <v>6.9</v>
       </c>
-      <c r="AE33" s="1" t="s">
+      <c r="AC33" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C34" s="1">
         <v>20201249</v>
@@ -4045,69 +3845,63 @@
         <v>9</v>
       </c>
       <c r="M34" s="1">
-        <v>0.1</v>
+        <v>22.4</v>
       </c>
       <c r="N34" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="O34" s="1">
-        <v>22.4</v>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="O34" s="3">
+        <v>79.648697758933977</v>
       </c>
       <c r="P34" s="1">
-        <v>2.5499999999999998</v>
+        <v>30.3</v>
       </c>
       <c r="Q34" s="1">
-        <v>1315</v>
+        <v>91.1</v>
       </c>
       <c r="R34" s="1">
-        <v>30.3</v>
+        <v>85.2</v>
       </c>
       <c r="S34" s="1">
-        <v>91.1</v>
+        <v>87.2</v>
       </c>
       <c r="T34" s="1">
-        <v>85.2</v>
+        <v>37.5</v>
       </c>
       <c r="U34" s="1">
-        <v>87.2</v>
+        <v>7.6</v>
       </c>
       <c r="V34" s="1">
-        <v>37.5</v>
+        <v>6.1</v>
       </c>
       <c r="W34" s="1">
-        <v>7.6</v>
-      </c>
-      <c r="X34" s="1">
-        <v>6.1</v>
+        <v>33.5</v>
+      </c>
+      <c r="X34" s="3">
+        <v>78.286475418859112</v>
       </c>
       <c r="Y34" s="1">
-        <v>33.5</v>
+        <v>12.7</v>
       </c>
       <c r="Z34" s="1">
-        <v>71117</v>
+        <v>78.41</v>
       </c>
       <c r="AA34" s="1">
-        <v>12.7</v>
+        <v>15.67</v>
       </c>
       <c r="AB34" s="1">
-        <v>78.41</v>
-      </c>
-      <c r="AC34" s="1">
-        <v>15.67</v>
-      </c>
-      <c r="AD34" s="1">
         <v>5.78</v>
       </c>
-      <c r="AE34" s="1" t="s">
+      <c r="AC34" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="1">
         <v>10439388</v>
@@ -4141,69 +3935,63 @@
         <v>3.2</v>
       </c>
       <c r="M35" s="1">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="N35" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O35" s="1">
-        <v>8</v>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="O35" s="3">
+        <v>56.450635978195031</v>
       </c>
       <c r="P35" s="1">
-        <v>2.5099999999999998</v>
+        <v>11.8</v>
       </c>
       <c r="Q35" s="1">
-        <v>932</v>
+        <v>90.7</v>
       </c>
       <c r="R35" s="1">
-        <v>11.8</v>
+        <v>83.4</v>
       </c>
       <c r="S35" s="1">
-        <v>90.7</v>
+        <v>88.5</v>
       </c>
       <c r="T35" s="1">
-        <v>83.4</v>
+        <v>32</v>
       </c>
       <c r="U35" s="1">
-        <v>88.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="V35" s="1">
-        <v>32</v>
+        <v>13.4</v>
       </c>
       <c r="W35" s="1">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="X35" s="1">
-        <v>13.4</v>
+        <v>24.9</v>
+      </c>
+      <c r="X35" s="3">
+        <v>62.352215935360299</v>
       </c>
       <c r="Y35" s="1">
-        <v>24.9</v>
+        <v>12.9</v>
       </c>
       <c r="Z35" s="1">
-        <v>56642</v>
+        <v>79.510000000000005</v>
       </c>
       <c r="AA35" s="1">
-        <v>12.9</v>
+        <v>14.4</v>
       </c>
       <c r="AB35" s="1">
-        <v>79.510000000000005</v>
-      </c>
-      <c r="AC35" s="1">
-        <v>14.4</v>
-      </c>
-      <c r="AD35" s="1">
         <v>5.93</v>
       </c>
-      <c r="AE35" s="1" t="s">
+      <c r="AC35" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="1">
         <v>779094</v>
@@ -4237,69 +4025,63 @@
         <v>1.7</v>
       </c>
       <c r="M36" s="1">
-        <v>0.1</v>
+        <v>4.3</v>
       </c>
       <c r="N36" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O36" s="1">
-        <v>4.3</v>
+        <v>2.29</v>
+      </c>
+      <c r="O36" s="3">
+        <v>50.151423379769831</v>
       </c>
       <c r="P36" s="1">
-        <v>2.29</v>
+        <v>6</v>
       </c>
       <c r="Q36" s="1">
-        <v>828</v>
+        <v>91.3</v>
       </c>
       <c r="R36" s="1">
-        <v>6</v>
+        <v>83.1</v>
       </c>
       <c r="S36" s="1">
-        <v>91.3</v>
+        <v>93.1</v>
       </c>
       <c r="T36" s="1">
-        <v>83.1</v>
+        <v>30.7</v>
       </c>
       <c r="U36" s="1">
-        <v>93.1</v>
+        <v>7.2</v>
       </c>
       <c r="V36" s="1">
-        <v>30.7</v>
+        <v>8.1</v>
       </c>
       <c r="W36" s="1">
-        <v>7.2</v>
-      </c>
-      <c r="X36" s="1">
-        <v>8.1</v>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="X36" s="3">
+        <v>71.899561876664976</v>
       </c>
       <c r="Y36" s="1">
-        <v>17.600000000000001</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="Z36" s="1">
-        <v>65315</v>
+        <v>72.819999999999993</v>
       </c>
       <c r="AA36" s="1">
-        <v>10.199999999999999</v>
+        <v>16.760000000000002</v>
       </c>
       <c r="AB36" s="1">
-        <v>72.819999999999993</v>
-      </c>
-      <c r="AC36" s="1">
-        <v>16.760000000000002</v>
-      </c>
-      <c r="AD36" s="1">
         <v>10.050000000000001</v>
       </c>
-      <c r="AE36" s="1" t="s">
+      <c r="AC36" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="1">
         <v>11799448</v>
@@ -4333,69 +4115,63 @@
         <v>2.5</v>
       </c>
       <c r="M37" s="1">
-        <v>0.1</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N37" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="O37" s="1">
-        <v>4.5999999999999996</v>
+        <v>2.41</v>
+      </c>
+      <c r="O37" s="3">
+        <v>49.969715324046035</v>
       </c>
       <c r="P37" s="1">
-        <v>2.41</v>
+        <v>7.2</v>
       </c>
       <c r="Q37" s="1">
-        <v>825</v>
+        <v>90.7</v>
       </c>
       <c r="R37" s="1">
-        <v>7.2</v>
+        <v>84.5</v>
       </c>
       <c r="S37" s="1">
-        <v>90.7</v>
+        <v>90.8</v>
       </c>
       <c r="T37" s="1">
-        <v>84.5</v>
+        <v>28.9</v>
       </c>
       <c r="U37" s="1">
-        <v>90.8</v>
+        <v>10</v>
       </c>
       <c r="V37" s="1">
-        <v>28.9</v>
+        <v>7.8</v>
       </c>
       <c r="W37" s="1">
-        <v>10</v>
-      </c>
-      <c r="X37" s="1">
-        <v>7.8</v>
+        <v>23.7</v>
+      </c>
+      <c r="X37" s="3">
+        <v>63.974813412298282</v>
       </c>
       <c r="Y37" s="1">
-        <v>23.7</v>
+        <v>12.6</v>
       </c>
       <c r="Z37" s="1">
-        <v>58116</v>
+        <v>83.15</v>
       </c>
       <c r="AA37" s="1">
-        <v>12.6</v>
+        <v>11.86</v>
       </c>
       <c r="AB37" s="1">
-        <v>83.15</v>
-      </c>
-      <c r="AC37" s="1">
-        <v>11.86</v>
-      </c>
-      <c r="AD37" s="1">
         <v>4.84</v>
       </c>
-      <c r="AE37" s="1" t="s">
+      <c r="AC37" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C38" s="1">
         <v>3959353</v>
@@ -4429,69 +4205,63 @@
         <v>2.4</v>
       </c>
       <c r="M38" s="1">
-        <v>0.2</v>
+        <v>6</v>
       </c>
       <c r="N38" s="1">
-        <v>6.3</v>
-      </c>
-      <c r="O38" s="1">
-        <v>6</v>
+        <v>2.57</v>
+      </c>
+      <c r="O38" s="3">
+        <v>49.545729860690493</v>
       </c>
       <c r="P38" s="1">
-        <v>2.57</v>
+        <v>10.6</v>
       </c>
       <c r="Q38" s="1">
-        <v>818</v>
+        <v>90.6</v>
       </c>
       <c r="R38" s="1">
-        <v>10.6</v>
+        <v>81.7</v>
       </c>
       <c r="S38" s="1">
-        <v>90.6</v>
+        <v>88.6</v>
       </c>
       <c r="T38" s="1">
-        <v>81.7</v>
+        <v>26.1</v>
       </c>
       <c r="U38" s="1">
-        <v>88.6</v>
+        <v>11.6</v>
       </c>
       <c r="V38" s="1">
-        <v>26.1</v>
+        <v>16.8</v>
       </c>
       <c r="W38" s="1">
-        <v>11.6</v>
-      </c>
-      <c r="X38" s="1">
-        <v>16.8</v>
+        <v>22</v>
+      </c>
+      <c r="X38" s="3">
+        <v>59.26773959181876</v>
       </c>
       <c r="Y38" s="1">
-        <v>22</v>
+        <v>14.3</v>
       </c>
       <c r="Z38" s="1">
-        <v>53840</v>
+        <v>76.760000000000005</v>
       </c>
       <c r="AA38" s="1">
-        <v>14.3</v>
+        <v>16.579999999999998</v>
       </c>
       <c r="AB38" s="1">
-        <v>76.760000000000005</v>
-      </c>
-      <c r="AC38" s="1">
-        <v>16.579999999999998</v>
-      </c>
-      <c r="AD38" s="1">
         <v>6.43</v>
       </c>
-      <c r="AE38" s="1" t="s">
+      <c r="AC38" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C39" s="1">
         <v>4237256</v>
@@ -4525,69 +4295,63 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="M39" s="1">
-        <v>0.5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="N39" s="1">
-        <v>4</v>
-      </c>
-      <c r="O39" s="1">
-        <v>9.8000000000000007</v>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="O39" s="3">
+        <v>71.047849788007269</v>
       </c>
       <c r="P39" s="1">
-        <v>2.4900000000000002</v>
+        <v>15.3</v>
       </c>
       <c r="Q39" s="1">
-        <v>1173</v>
+        <v>94.1</v>
       </c>
       <c r="R39" s="1">
-        <v>15.3</v>
+        <v>88.1</v>
       </c>
       <c r="S39" s="1">
-        <v>94.1</v>
+        <v>91.1</v>
       </c>
       <c r="T39" s="1">
-        <v>88.1</v>
+        <v>34.4</v>
       </c>
       <c r="U39" s="1">
-        <v>91.1</v>
+        <v>9.9</v>
       </c>
       <c r="V39" s="1">
-        <v>34.4</v>
+        <v>8.6</v>
       </c>
       <c r="W39" s="1">
-        <v>9.9</v>
-      </c>
-      <c r="X39" s="1">
-        <v>8.6</v>
+        <v>23.9</v>
+      </c>
+      <c r="X39" s="3">
+        <v>72.287047841306887</v>
       </c>
       <c r="Y39" s="1">
-        <v>23.9</v>
+        <v>11</v>
       </c>
       <c r="Z39" s="1">
-        <v>65667</v>
+        <v>77.72</v>
       </c>
       <c r="AA39" s="1">
-        <v>11</v>
+        <v>14.17</v>
       </c>
       <c r="AB39" s="1">
-        <v>77.72</v>
-      </c>
-      <c r="AC39" s="1">
-        <v>14.17</v>
-      </c>
-      <c r="AD39" s="1">
         <v>7.9</v>
       </c>
-      <c r="AE39" s="1" t="s">
+      <c r="AC39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C40" s="1">
         <v>13002700</v>
@@ -4621,69 +4385,63 @@
         <v>3.8</v>
       </c>
       <c r="M40" s="1">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="N40" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="O40" s="1">
+        <v>2.42</v>
+      </c>
+      <c r="O40" s="3">
+        <v>58.025439127801334</v>
+      </c>
+      <c r="P40" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>89.6</v>
+      </c>
+      <c r="R40" s="1">
+        <v>84</v>
+      </c>
+      <c r="S40" s="1">
+        <v>91</v>
+      </c>
+      <c r="T40" s="1">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="U40" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="V40" s="1">
         <v>7</v>
       </c>
-      <c r="P40" s="1">
-        <v>2.42</v>
-      </c>
-      <c r="Q40" s="1">
-        <v>958</v>
-      </c>
-      <c r="R40" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="S40" s="1">
-        <v>89.6</v>
-      </c>
-      <c r="T40" s="1">
-        <v>84</v>
-      </c>
-      <c r="U40" s="1">
-        <v>91</v>
-      </c>
-      <c r="V40" s="1">
-        <v>32.299999999999997</v>
-      </c>
       <c r="W40" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="X40" s="1">
-        <v>7</v>
+        <v>27.1</v>
+      </c>
+      <c r="X40" s="3">
+        <v>70.041390546223113</v>
       </c>
       <c r="Y40" s="1">
-        <v>27.1</v>
+        <v>10.9</v>
       </c>
       <c r="Z40" s="1">
-        <v>63627</v>
+        <v>84.39</v>
       </c>
       <c r="AA40" s="1">
-        <v>10.9</v>
+        <v>10.43</v>
       </c>
       <c r="AB40" s="1">
-        <v>84.39</v>
-      </c>
-      <c r="AC40" s="1">
-        <v>10.43</v>
-      </c>
-      <c r="AD40" s="1">
         <v>5.04</v>
       </c>
-      <c r="AE40" s="1" t="s">
+      <c r="AC40" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C41" s="1">
         <v>1097379</v>
@@ -4717,69 +4475,63 @@
         <v>3.7</v>
       </c>
       <c r="M41" s="1">
-        <v>0.2</v>
+        <v>14</v>
       </c>
       <c r="N41" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="O41" s="1">
-        <v>14</v>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="O41" s="3">
+        <v>62.447001817080562</v>
       </c>
       <c r="P41" s="1">
-        <v>2.4500000000000002</v>
+        <v>22.4</v>
       </c>
       <c r="Q41" s="1">
-        <v>1031</v>
+        <v>90.7</v>
       </c>
       <c r="R41" s="1">
-        <v>22.4</v>
+        <v>86.6</v>
       </c>
       <c r="S41" s="1">
-        <v>90.7</v>
+        <v>89.2</v>
       </c>
       <c r="T41" s="1">
-        <v>86.6</v>
+        <v>35</v>
       </c>
       <c r="U41" s="1">
-        <v>89.2</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="V41" s="1">
-        <v>35</v>
+        <v>4.8</v>
       </c>
       <c r="W41" s="1">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="X41" s="1">
-        <v>4.8</v>
+        <v>25.3</v>
+      </c>
+      <c r="X41" s="3">
+        <v>77.392615750423815</v>
       </c>
       <c r="Y41" s="1">
-        <v>25.3</v>
+        <v>10.6</v>
       </c>
       <c r="Z41" s="1">
-        <v>70305</v>
+        <v>82.78</v>
       </c>
       <c r="AA41" s="1">
-        <v>10.6</v>
+        <v>12.09</v>
       </c>
       <c r="AB41" s="1">
-        <v>82.78</v>
-      </c>
-      <c r="AC41" s="1">
-        <v>12.09</v>
-      </c>
-      <c r="AD41" s="1">
         <v>5.04</v>
       </c>
-      <c r="AE41" s="1" t="s">
+      <c r="AC41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C42" s="1">
         <v>5118425</v>
@@ -4813,69 +4565,63 @@
         <v>1.8</v>
       </c>
       <c r="M42" s="1">
-        <v>0.1</v>
+        <v>5.2</v>
       </c>
       <c r="N42" s="1">
-        <v>2</v>
-      </c>
-      <c r="O42" s="1">
-        <v>5.2</v>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="O42" s="3">
+        <v>55.602665051483946</v>
       </c>
       <c r="P42" s="1">
-        <v>2.5299999999999998</v>
+        <v>7.4</v>
       </c>
       <c r="Q42" s="1">
-        <v>918</v>
+        <v>90.2</v>
       </c>
       <c r="R42" s="1">
-        <v>7.4</v>
+        <v>81.2</v>
       </c>
       <c r="S42" s="1">
-        <v>90.2</v>
+        <v>88.3</v>
       </c>
       <c r="T42" s="1">
-        <v>81.2</v>
+        <v>29</v>
       </c>
       <c r="U42" s="1">
-        <v>88.3</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="V42" s="1">
-        <v>29</v>
+        <v>13.2</v>
       </c>
       <c r="W42" s="1">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="X42" s="1">
-        <v>13.2</v>
+        <v>25.1</v>
+      </c>
+      <c r="X42" s="3">
+        <v>60.394971488958845</v>
       </c>
       <c r="Y42" s="1">
-        <v>25.1</v>
+        <v>13.8</v>
       </c>
       <c r="Z42" s="1">
-        <v>54864</v>
+        <v>79.23</v>
       </c>
       <c r="AA42" s="1">
-        <v>13.8</v>
+        <v>15.33</v>
       </c>
       <c r="AB42" s="1">
-        <v>79.23</v>
-      </c>
-      <c r="AC42" s="1">
-        <v>15.33</v>
-      </c>
-      <c r="AD42" s="1">
         <v>5.28</v>
       </c>
-      <c r="AE42" s="1" t="s">
+      <c r="AC42" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C43" s="1">
         <v>886667</v>
@@ -4909,69 +4655,63 @@
         <v>1.5</v>
       </c>
       <c r="M43" s="1">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="N43" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="O43" s="1">
-        <v>4</v>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="O43" s="3">
+        <v>46.093276801938224</v>
       </c>
       <c r="P43" s="1">
-        <v>2.4300000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="Q43" s="1">
-        <v>761</v>
+        <v>90.2</v>
       </c>
       <c r="R43" s="1">
-        <v>6.5</v>
+        <v>83.2</v>
       </c>
       <c r="S43" s="1">
-        <v>90.2</v>
+        <v>92.2</v>
       </c>
       <c r="T43" s="1">
-        <v>83.2</v>
+        <v>29.3</v>
       </c>
       <c r="U43" s="1">
-        <v>92.2</v>
+        <v>7.8</v>
       </c>
       <c r="V43" s="1">
-        <v>29.3</v>
+        <v>12.2</v>
       </c>
       <c r="W43" s="1">
-        <v>7.8</v>
-      </c>
-      <c r="X43" s="1">
-        <v>12.2</v>
+        <v>17.3</v>
+      </c>
+      <c r="X43" s="3">
+        <v>65.93425948349882</v>
       </c>
       <c r="Y43" s="1">
-        <v>17.3</v>
+        <v>11.6</v>
       </c>
       <c r="Z43" s="1">
-        <v>59896</v>
+        <v>72.75</v>
       </c>
       <c r="AA43" s="1">
-        <v>11.6</v>
+        <v>16.79</v>
       </c>
       <c r="AB43" s="1">
-        <v>72.75</v>
-      </c>
-      <c r="AC43" s="1">
-        <v>16.79</v>
-      </c>
-      <c r="AD43" s="1">
         <v>10.01</v>
       </c>
-      <c r="AE43" s="1" t="s">
+      <c r="AC43" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C44" s="1">
         <v>6910840</v>
@@ -5005,69 +4745,63 @@
         <v>2</v>
       </c>
       <c r="M44" s="1">
-        <v>0.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="N44" s="1">
-        <v>2</v>
-      </c>
-      <c r="O44" s="1">
-        <v>5.0999999999999996</v>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="O44" s="3">
+        <v>54.330708661417326</v>
       </c>
       <c r="P44" s="1">
-        <v>2.5099999999999998</v>
+        <v>7.2</v>
       </c>
       <c r="Q44" s="1">
-        <v>897</v>
+        <v>89.1</v>
       </c>
       <c r="R44" s="1">
-        <v>7.2</v>
+        <v>81.5</v>
       </c>
       <c r="S44" s="1">
-        <v>89.1</v>
+        <v>88.2</v>
       </c>
       <c r="T44" s="1">
-        <v>81.5</v>
+        <v>28.2</v>
       </c>
       <c r="U44" s="1">
-        <v>88.2</v>
+        <v>11</v>
       </c>
       <c r="V44" s="1">
-        <v>28.2</v>
+        <v>12.1</v>
       </c>
       <c r="W44" s="1">
-        <v>11</v>
-      </c>
-      <c r="X44" s="1">
-        <v>12.1</v>
+        <v>25.4</v>
+      </c>
+      <c r="X44" s="3">
+        <v>60.360846304572782</v>
       </c>
       <c r="Y44" s="1">
-        <v>25.4</v>
+        <v>13.6</v>
       </c>
       <c r="Z44" s="1">
-        <v>54833</v>
+        <v>79.02</v>
       </c>
       <c r="AA44" s="1">
-        <v>13.6</v>
+        <v>13.92</v>
       </c>
       <c r="AB44" s="1">
-        <v>79.02</v>
-      </c>
-      <c r="AC44" s="1">
-        <v>13.92</v>
-      </c>
-      <c r="AD44" s="1">
         <v>6.89</v>
       </c>
-      <c r="AE44" s="1" t="s">
+      <c r="AC44" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C45" s="1">
         <v>29145505</v>
@@ -5101,69 +4835,63 @@
         <v>5.2</v>
       </c>
       <c r="M45" s="1">
-        <v>0.1</v>
+        <v>16.8</v>
       </c>
       <c r="N45" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="O45" s="1">
-        <v>16.8</v>
+        <v>2.83</v>
+      </c>
+      <c r="O45" s="3">
+        <v>65.536038764385225</v>
       </c>
       <c r="P45" s="1">
-        <v>2.83</v>
+        <v>35.1</v>
       </c>
       <c r="Q45" s="1">
-        <v>1082</v>
+        <v>92.7</v>
       </c>
       <c r="R45" s="1">
-        <v>35.1</v>
+        <v>85.1</v>
       </c>
       <c r="S45" s="1">
-        <v>92.7</v>
+        <v>84.4</v>
       </c>
       <c r="T45" s="1">
-        <v>85.1</v>
+        <v>30.7</v>
       </c>
       <c r="U45" s="1">
-        <v>84.4</v>
+        <v>7.9</v>
       </c>
       <c r="V45" s="1">
-        <v>30.7</v>
+        <v>20.8</v>
       </c>
       <c r="W45" s="1">
-        <v>7.9</v>
-      </c>
-      <c r="X45" s="1">
-        <v>20.8</v>
+        <v>26.6</v>
+      </c>
+      <c r="X45" s="3">
+        <v>70.260452213733743</v>
       </c>
       <c r="Y45" s="1">
-        <v>26.6</v>
+        <v>13.4</v>
       </c>
       <c r="Z45" s="1">
-        <v>63826</v>
+        <v>79.37</v>
       </c>
       <c r="AA45" s="1">
-        <v>13.4</v>
+        <v>13.48</v>
       </c>
       <c r="AB45" s="1">
-        <v>79.37</v>
-      </c>
-      <c r="AC45" s="1">
-        <v>13.48</v>
-      </c>
-      <c r="AD45" s="1">
         <v>6.97</v>
       </c>
-      <c r="AE45" s="1" t="s">
+      <c r="AC45" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C46" s="1">
         <v>3271616</v>
@@ -5197,69 +4925,63 @@
         <v>2.7</v>
       </c>
       <c r="M46" s="1">
-        <v>1.1000000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="N46" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="O46" s="1">
-        <v>8.4</v>
+        <v>3.09</v>
+      </c>
+      <c r="O46" s="3">
+        <v>66.020593579648704</v>
       </c>
       <c r="P46" s="1">
-        <v>3.09</v>
+        <v>15.3</v>
       </c>
       <c r="Q46" s="1">
-        <v>1090</v>
+        <v>96.1</v>
       </c>
       <c r="R46" s="1">
-        <v>15.3</v>
+        <v>89.3</v>
       </c>
       <c r="S46" s="1">
-        <v>96.1</v>
+        <v>93</v>
       </c>
       <c r="T46" s="1">
-        <v>89.3</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="U46" s="1">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="V46" s="1">
-        <v>34.700000000000003</v>
+        <v>10.8</v>
       </c>
       <c r="W46" s="1">
-        <v>7</v>
-      </c>
-      <c r="X46" s="1">
-        <v>10.8</v>
+        <v>22</v>
+      </c>
+      <c r="X46" s="3">
+        <v>81.676977609475799</v>
       </c>
       <c r="Y46" s="1">
-        <v>22</v>
+        <v>7.3</v>
       </c>
       <c r="Z46" s="1">
-        <v>74197</v>
+        <v>80.260000000000005</v>
       </c>
       <c r="AA46" s="1">
-        <v>7.3</v>
+        <v>14.76</v>
       </c>
       <c r="AB46" s="1">
-        <v>80.260000000000005</v>
-      </c>
-      <c r="AC46" s="1">
-        <v>14.76</v>
-      </c>
-      <c r="AD46" s="1">
         <v>4.82</v>
       </c>
-      <c r="AE46" s="1" t="s">
+      <c r="AC46" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C47" s="1">
         <v>643077</v>
@@ -5293,69 +5015,63 @@
         <v>1.9</v>
       </c>
       <c r="M47" s="1">
-        <v>0.1</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N47" s="1">
-        <v>2</v>
-      </c>
-      <c r="O47" s="1">
-        <v>4.5999999999999996</v>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="O47" s="3">
+        <v>60.508782556026652</v>
       </c>
       <c r="P47" s="1">
-        <v>2.2799999999999998</v>
+        <v>5.6</v>
       </c>
       <c r="Q47" s="1">
-        <v>999</v>
+        <v>91.3</v>
       </c>
       <c r="R47" s="1">
+        <v>83</v>
+      </c>
+      <c r="S47" s="1">
+        <v>93.5</v>
+      </c>
+      <c r="T47" s="1">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="U47" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="V47" s="1">
         <v>5.6</v>
       </c>
-      <c r="S47" s="1">
-        <v>91.3</v>
-      </c>
-      <c r="T47" s="1">
-        <v>83</v>
-      </c>
-      <c r="U47" s="1">
-        <v>93.5</v>
-      </c>
-      <c r="V47" s="1">
-        <v>39.700000000000003</v>
-      </c>
       <c r="W47" s="1">
-        <v>10.4</v>
-      </c>
-      <c r="X47" s="1">
-        <v>5.6</v>
+        <v>23.3</v>
+      </c>
+      <c r="X47" s="3">
+        <v>69.876268686290473</v>
       </c>
       <c r="Y47" s="1">
-        <v>23.3</v>
+        <v>9.4</v>
       </c>
       <c r="Z47" s="1">
-        <v>63477</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="AA47" s="1">
-        <v>9.4</v>
+        <v>14.12</v>
       </c>
       <c r="AB47" s="1">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="AC47" s="1">
-        <v>14.12</v>
-      </c>
-      <c r="AD47" s="1">
         <v>9.49</v>
       </c>
-      <c r="AE47" s="1" t="s">
+      <c r="AC47" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C48" s="1">
         <v>8631393</v>
@@ -5389,69 +5105,63 @@
         <v>6.9</v>
       </c>
       <c r="M48" s="1">
-        <v>0.1</v>
+        <v>12.6</v>
       </c>
       <c r="N48" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="O48" s="1">
-        <v>12.6</v>
+        <v>2.6</v>
+      </c>
+      <c r="O48" s="3">
+        <v>76.135675348273764</v>
       </c>
       <c r="P48" s="1">
-        <v>2.6</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="Q48" s="1">
-        <v>1257</v>
+        <v>92.3</v>
       </c>
       <c r="R48" s="1">
-        <v>16.399999999999999</v>
+        <v>86.1</v>
       </c>
       <c r="S48" s="1">
-        <v>92.3</v>
+        <v>90.3</v>
       </c>
       <c r="T48" s="1">
-        <v>86.1</v>
+        <v>39.5</v>
       </c>
       <c r="U48" s="1">
-        <v>90.3</v>
+        <v>8</v>
       </c>
       <c r="V48" s="1">
-        <v>39.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="W48" s="1">
-        <v>8</v>
-      </c>
-      <c r="X48" s="1">
-        <v>9.3000000000000007</v>
+        <v>28.6</v>
+      </c>
+      <c r="X48" s="3">
+        <v>84.09986570088725</v>
       </c>
       <c r="Y48" s="1">
-        <v>28.6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="Z48" s="1">
-        <v>76398</v>
+        <v>74.760000000000005</v>
       </c>
       <c r="AA48" s="1">
-        <v>9.1999999999999993</v>
+        <v>20.13</v>
       </c>
       <c r="AB48" s="1">
-        <v>74.760000000000005</v>
-      </c>
-      <c r="AC48" s="1">
-        <v>20.13</v>
-      </c>
-      <c r="AD48" s="1">
         <v>4.96</v>
       </c>
-      <c r="AE48" s="1" t="s">
+      <c r="AC48" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1">
         <v>7705281</v>
@@ -5485,69 +5195,63 @@
         <v>9.6</v>
       </c>
       <c r="M49" s="1">
-        <v>0.8</v>
+        <v>14.5</v>
       </c>
       <c r="N49" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O49" s="1">
-        <v>14.5</v>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="O49" s="3">
+        <v>80.981223500908541</v>
       </c>
       <c r="P49" s="1">
-        <v>2.5299999999999998</v>
+        <v>20</v>
       </c>
       <c r="Q49" s="1">
-        <v>1337</v>
+        <v>94.8</v>
       </c>
       <c r="R49" s="1">
-        <v>20</v>
+        <v>90.1</v>
       </c>
       <c r="S49" s="1">
-        <v>94.8</v>
+        <v>91.7</v>
       </c>
       <c r="T49" s="1">
-        <v>90.1</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="U49" s="1">
-        <v>91.7</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="V49" s="1">
-        <v>36.700000000000003</v>
+        <v>7.7</v>
       </c>
       <c r="W49" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="X49" s="1">
-        <v>7.7</v>
+        <v>28</v>
+      </c>
+      <c r="X49" s="3">
+        <v>84.769159639814191</v>
       </c>
       <c r="Y49" s="1">
-        <v>28</v>
+        <v>9.5</v>
       </c>
       <c r="Z49" s="1">
-        <v>77006</v>
+        <v>76.989999999999995</v>
       </c>
       <c r="AA49" s="1">
-        <v>9.5</v>
+        <v>16.75</v>
       </c>
       <c r="AB49" s="1">
-        <v>76.989999999999995</v>
-      </c>
-      <c r="AC49" s="1">
-        <v>16.75</v>
-      </c>
-      <c r="AD49" s="1">
         <v>6.08</v>
       </c>
-      <c r="AE49" s="1" t="s">
+      <c r="AC49" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C50" s="1">
         <v>1793716</v>
@@ -5581,69 +5285,63 @@
         <v>0.8</v>
       </c>
       <c r="M50" s="1">
-        <v>0.1</v>
+        <v>1.6</v>
       </c>
       <c r="N50" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="O50" s="1">
-        <v>1.6</v>
+        <v>2.5</v>
+      </c>
+      <c r="O50" s="3">
+        <v>44.336765596608117</v>
       </c>
       <c r="P50" s="1">
         <v>2.5</v>
       </c>
       <c r="Q50" s="1">
-        <v>732</v>
+        <v>86.2</v>
       </c>
       <c r="R50" s="1">
-        <v>2.5</v>
+        <v>78.900000000000006</v>
       </c>
       <c r="S50" s="1">
-        <v>86.2</v>
+        <v>87.6</v>
       </c>
       <c r="T50" s="1">
-        <v>78.900000000000006</v>
+        <v>21.3</v>
       </c>
       <c r="U50" s="1">
-        <v>87.6</v>
+        <v>13.9</v>
       </c>
       <c r="V50" s="1">
-        <v>21.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="W50" s="1">
-        <v>13.9</v>
-      </c>
-      <c r="X50" s="1">
-        <v>8.3000000000000007</v>
+        <v>26.1</v>
+      </c>
+      <c r="X50" s="3">
+        <v>52.879725237225074</v>
       </c>
       <c r="Y50" s="1">
-        <v>26.1</v>
+        <v>15.8</v>
       </c>
       <c r="Z50" s="1">
-        <v>48037</v>
+        <v>76.87</v>
       </c>
       <c r="AA50" s="1">
-        <v>15.8</v>
+        <v>18.64</v>
       </c>
       <c r="AB50" s="1">
-        <v>76.87</v>
-      </c>
-      <c r="AC50" s="1">
-        <v>18.64</v>
-      </c>
-      <c r="AD50" s="1">
         <v>4.37</v>
       </c>
-      <c r="AE50" s="1" t="s">
+      <c r="AC50" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1">
         <v>5893718</v>
@@ -5677,69 +5375,63 @@
         <v>3</v>
       </c>
       <c r="M51" s="1">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="N51" s="1">
-        <v>2</v>
-      </c>
-      <c r="O51" s="1">
-        <v>5</v>
+        <v>2.38</v>
+      </c>
+      <c r="O51" s="3">
+        <v>52.816474863718952</v>
       </c>
       <c r="P51" s="1">
-        <v>2.38</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Q51" s="1">
-        <v>872</v>
+        <v>90.7</v>
       </c>
       <c r="R51" s="1">
-        <v>8.6999999999999993</v>
+        <v>84.7</v>
       </c>
       <c r="S51" s="1">
-        <v>90.7</v>
+        <v>92.6</v>
       </c>
       <c r="T51" s="1">
-        <v>84.7</v>
+        <v>30.8</v>
       </c>
       <c r="U51" s="1">
-        <v>92.6</v>
+        <v>8</v>
       </c>
       <c r="V51" s="1">
-        <v>30.8</v>
+        <v>6.8</v>
       </c>
       <c r="W51" s="1">
-        <v>8</v>
-      </c>
-      <c r="X51" s="1">
-        <v>6.8</v>
+        <v>22.2</v>
+      </c>
+      <c r="X51" s="3">
+        <v>69.673719204773121</v>
       </c>
       <c r="Y51" s="1">
-        <v>22.2</v>
+        <v>10</v>
       </c>
       <c r="Z51" s="1">
-        <v>63293</v>
+        <v>82.47</v>
       </c>
       <c r="AA51" s="1">
-        <v>10</v>
+        <v>12.09</v>
       </c>
       <c r="AB51" s="1">
-        <v>82.47</v>
-      </c>
-      <c r="AC51" s="1">
-        <v>12.09</v>
-      </c>
-      <c r="AD51" s="1">
         <v>5.24</v>
       </c>
-      <c r="AE51" s="1" t="s">
+      <c r="AC51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1">
         <v>576851</v>
@@ -5773,60 +5465,54 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M52" s="1">
-        <v>0.1</v>
+        <v>3.3</v>
       </c>
       <c r="N52" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O52" s="1">
-        <v>3.3</v>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="O52" s="3">
+        <v>51.665657177468205</v>
       </c>
       <c r="P52" s="1">
-        <v>2.4300000000000002</v>
+        <v>7</v>
       </c>
       <c r="Q52" s="1">
-        <v>853</v>
+        <v>93.1</v>
       </c>
       <c r="R52" s="1">
-        <v>7</v>
+        <v>85.9</v>
       </c>
       <c r="S52" s="1">
-        <v>93.1</v>
+        <v>93.6</v>
       </c>
       <c r="T52" s="1">
-        <v>85.9</v>
+        <v>28.2</v>
       </c>
       <c r="U52" s="1">
-        <v>93.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="V52" s="1">
-        <v>28.2</v>
+        <v>14.8</v>
       </c>
       <c r="W52" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="X52" s="1">
-        <v>14.8</v>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="X52" s="3">
+        <v>71.887452940269924</v>
       </c>
       <c r="Y52" s="1">
-        <v>17.899999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="Z52" s="1">
-        <v>65304</v>
+        <v>71.25</v>
       </c>
       <c r="AA52" s="1">
-        <v>9.1999999999999993</v>
+        <v>21.75</v>
       </c>
       <c r="AB52" s="1">
-        <v>71.25</v>
-      </c>
-      <c r="AC52" s="1">
-        <v>21.75</v>
-      </c>
-      <c r="AD52" s="1">
         <v>6.68</v>
       </c>
-      <c r="AE52" s="1" t="s">
+      <c r="AC52" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>